<commit_message>
Update of the list
</commit_message>
<xml_diff>
--- a/Data/DS courses list.xlsx
+++ b/Data/DS courses list.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ola\OneDrive - Universiteit Utrecht\Documents\GitHub\UU-DS-courses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ola\OneDrive - Universiteit Utrecht\Documents\GitHub\UU-DS-courses\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424984F1-6DBD-42DE-B44B-B20C9D388A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C279FF1-E592-4FC1-8C22-BD717C3E6CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1526A550-0408-4384-9B3B-2B5C51FB6CCB}"/>
+    <workbookView xWindow="1545" yWindow="-12765" windowWidth="28965" windowHeight="11730" xr2:uid="{1526A550-0408-4384-9B3B-2B5C51FB6CCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AY$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AZ$53</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,9 +46,19 @@
     <author>tc={2C1CB73F-0B60-41E5-AECE-1427034B9CE3}</author>
     <author>tc={35885A4E-3B89-4D6A-95CD-08862DFB9430}</author>
     <author>tc={0477E9A7-5E83-41B8-965E-BC68BE4572C4}</author>
+    <author>tc={E2FFAAF8-7744-465F-9701-9A2AFF0D8FD2}</author>
+    <author>tc={971B0614-288D-4052-BBD0-23AC10C52401}</author>
+    <author>tc={7C5818E2-1E6A-4677-95FD-D0E0F1BC44BF}</author>
+    <author>tc={0F9D3427-B4EC-4231-A8B8-1CD7AE2C5236}</author>
+    <author>tc={B346AB8C-D5F8-4A60-B1CA-15714598AC1D}</author>
+    <author>tc={FA9CD2C0-F5EE-473A-BF68-EE1E51FD7EED}</author>
+    <author>tc={74E5C956-2E55-47CF-908B-6DF2CA8BFF70}</author>
+    <author>tc={D9A68AAD-F7F5-48E9-86BF-E791855CE074}</author>
+    <author>tc={D2CE96B7-DA8C-4491-9962-80A041D6783C}</author>
+    <author>tc={0156854D-B856-40C8-9F6A-56D1A73DF7D0}</author>
   </authors>
   <commentList>
-    <comment ref="AN1" authorId="0" shapeId="0" xr:uid="{7912B0EA-387D-478B-95D3-9090A6112730}">
+    <comment ref="AO1" authorId="0" shapeId="0" xr:uid="{7912B0EA-387D-478B-95D3-9090A6112730}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -57,7 +67,7 @@
 INFOMEBD: developing and validating clinical prediction models using IPD</t>
       </text>
     </comment>
-    <comment ref="AN26" authorId="1" shapeId="0" xr:uid="{235018C0-EEF6-44A5-9ED8-1B80DA82E322}">
+    <comment ref="AO26" authorId="1" shapeId="0" xr:uid="{235018C0-EEF6-44A5-9ED8-1B80DA82E322}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -65,7 +75,7 @@
     probability</t>
       </text>
     </comment>
-    <comment ref="AT26" authorId="2" shapeId="0" xr:uid="{55636430-28F9-427E-8FC9-0523E795980C}">
+    <comment ref="AU26" authorId="2" shapeId="0" xr:uid="{55636430-28F9-427E-8FC9-0523E795980C}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -83,7 +93,7 @@
 sparse recovery</t>
       </text>
     </comment>
-    <comment ref="AN30" authorId="3" shapeId="0" xr:uid="{4D3D460E-D00C-48E4-97F6-28235A8C037F}">
+    <comment ref="AO30" authorId="3" shapeId="0" xr:uid="{4D3D460E-D00C-48E4-97F6-28235A8C037F}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -99,7 +109,7 @@
 Fitted values</t>
       </text>
     </comment>
-    <comment ref="AN31" authorId="4" shapeId="0" xr:uid="{2C1CB73F-0B60-41E5-AECE-1427034B9CE3}">
+    <comment ref="AO31" authorId="4" shapeId="0" xr:uid="{2C1CB73F-0B60-41E5-AECE-1427034B9CE3}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -115,7 +125,7 @@
     The course covers the essentials of qualitative research, in particular techniques for identifying themes, the making of systematic comparisons, and grounding interpretation in theory. Finally, it focuses on the principles of dovetailing primary ethnographic research, secondary data, and larger theoretical frames.</t>
       </text>
     </comment>
-    <comment ref="AN49" authorId="6" shapeId="0" xr:uid="{0477E9A7-5E83-41B8-965E-BC68BE4572C4}">
+    <comment ref="AO49" authorId="6" shapeId="0" xr:uid="{0477E9A7-5E83-41B8-965E-BC68BE4572C4}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -123,12 +133,94 @@
     inference</t>
       </text>
     </comment>
+    <comment ref="A55" authorId="7" shapeId="0" xr:uid="{E2FFAAF8-7744-465F-9701-9A2AFF0D8FD2}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    This course mentions in discription a statistical software use but I'm not sure what it is</t>
+      </text>
+    </comment>
+    <comment ref="AR62" authorId="8" shapeId="0" xr:uid="{971B0614-288D-4052-BBD0-23AC10C52401}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    qualitative data</t>
+      </text>
+    </comment>
+    <comment ref="AU62" authorId="9" shapeId="0" xr:uid="{7C5818E2-1E6A-4677-95FD-D0E0F1BC44BF}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</t>
+      </text>
+    </comment>
+    <comment ref="A63" authorId="10" shapeId="0" xr:uid="{0F9D3427-B4EC-4231-A8B8-1CD7AE2C5236}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    no course description
+Odpowiedź:
+    only spss mantioned in the literature</t>
+      </text>
+    </comment>
+    <comment ref="AR64" authorId="11" shapeId="0" xr:uid="{B346AB8C-D5F8-4A60-B1CA-15714598AC1D}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    qualitative data</t>
+      </text>
+    </comment>
+    <comment ref="AU64" authorId="12" shapeId="0" xr:uid="{FA9CD2C0-F5EE-473A-BF68-EE1E51FD7EED}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</t>
+      </text>
+    </comment>
+    <comment ref="AR65" authorId="13" shapeId="0" xr:uid="{74E5C956-2E55-47CF-908B-6DF2CA8BFF70}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    qualitative data</t>
+      </text>
+    </comment>
+    <comment ref="AU65" authorId="14" shapeId="0" xr:uid="{D9A68AAD-F7F5-48E9-86BF-E791855CE074}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</t>
+      </text>
+    </comment>
+    <comment ref="AR66" authorId="15" shapeId="0" xr:uid="{D2CE96B7-DA8C-4491-9962-80A041D6783C}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</t>
+      </text>
+    </comment>
+    <comment ref="AU66" authorId="16" shapeId="0" xr:uid="{0156854D-B856-40C8-9F6A-56D1A73DF7D0}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="307">
   <si>
     <t>Course Name</t>
   </si>
@@ -282,9 +374,6 @@
     <t>Epi</t>
   </si>
   <si>
-    <t> statistical methods</t>
-  </si>
-  <si>
     <t>INFOMUDR</t>
   </si>
   <si>
@@ -423,9 +512,6 @@
     <t>Database management</t>
   </si>
   <si>
-    <t>data collection</t>
-  </si>
-  <si>
     <t>Data analytics</t>
   </si>
   <si>
@@ -486,9 +572,6 @@
     <t>Applied Data Science Profile (PROFILE-ADS), Business Informatics (MBIM)</t>
   </si>
   <si>
-    <t xml:space="preserve">data science practice awarenes and ethics </t>
-  </si>
-  <si>
     <t>nonSQL databases</t>
   </si>
   <si>
@@ -931,13 +1014,163 @@
   </si>
   <si>
     <t>S005</t>
+  </si>
+  <si>
+    <t>ADS: Foundation of Research and Statistics</t>
+  </si>
+  <si>
+    <t>MSc. H.J. Leplaa</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>not Academische lerarenopleiding primair onderwijs, not Cultural Anthropology and Development Sociology, not Educational Sciences, not Interdisciplinary Social Sciences, not Pedagogical Sciences, not Psychology, not Sociology</t>
+  </si>
+  <si>
+    <t>Bayesian statistics</t>
+  </si>
+  <si>
+    <t> statistical methods (non bayesian)</t>
+  </si>
+  <si>
+    <t>Advanced Research Methods and Statistics for Psychology</t>
+  </si>
+  <si>
+    <t>prof. dr. I.G. Klugkist</t>
+  </si>
+  <si>
+    <t>MSc. A.F. ten Brink, dr. M.J. van der Smagt, dr. S. Gayet, dr. T. van Timmeren</t>
+  </si>
+  <si>
+    <t>KOM (201800051), TOE (201800055)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advanced Sociological Theory: Modelling Social Interaction </t>
+  </si>
+  <si>
+    <t>Only for students from Keulen/Mannheim! This course is a 6 week program.</t>
+  </si>
+  <si>
+    <t>dr. R. Corten</t>
+  </si>
+  <si>
+    <t>Advanced Sociological Theory: Modelling Social interaction </t>
+  </si>
+  <si>
+    <t>dr. R. Corten, prof. dr. ir. V.W. Buskens, MSc. A. Macanović, dr. D. Mazrekaj, dr. M. Kros</t>
+  </si>
+  <si>
+    <t>dr. R. Corten, prof. dr. ir. V.W. Buskens, MSc. A. Macanović, dr. D. Mazrekaj, dr. M. Kros, W.B.P. Kwint</t>
+  </si>
+  <si>
+    <t>Sociology and social research (SW-SOC-MI5), Sociology: Contemporary Social Problems (SW-SOC-MI6)</t>
+  </si>
+  <si>
+    <t>Advanced Statistics II: Introduction in multilevel and structural equation modelling for EdSci</t>
+  </si>
+  <si>
+    <t>dr. L.D.N.V. Wijngaards</t>
+  </si>
+  <si>
+    <t>Educational Sciences: Learning in Interaction (EDSM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strong theoretical base of data science practice and ethics </t>
+  </si>
+  <si>
+    <t>HLM</t>
+  </si>
+  <si>
+    <t>Advanced research methods and statistics for Interdisciplinary Social Sciences </t>
+  </si>
+  <si>
+    <t>dr. C. Rietbergen</t>
+  </si>
+  <si>
+    <t>dr. Duco Veen</t>
+  </si>
+  <si>
+    <t>Liberal Arts and Sciences (LASB)</t>
+  </si>
+  <si>
+    <t>Liberal Arts and Sciences (LASB),  Social Education and Youth Policy (SW-PED-MI12)</t>
+  </si>
+  <si>
+    <t>Advanced research methods and statistics for pedagogical sciences</t>
+  </si>
+  <si>
+    <t>dr. ir. N.W. Lagerweij</t>
+  </si>
+  <si>
+    <t>KOM (201800051), TOE (201800055), BOS</t>
+  </si>
+  <si>
+    <t>Advanced statistics I: Multivariate statistics in practice for EdSci</t>
+  </si>
+  <si>
+    <t>dr. M. Moerbeek</t>
+  </si>
+  <si>
+    <t>dr. L.D.N.V. Wijngaards, dr. E.M. Grandfield, prof. dr. Tamara van Gog</t>
+  </si>
+  <si>
+    <t>prof. dr. Tamara van Gog</t>
+  </si>
+  <si>
+    <t>Text mining</t>
+  </si>
+  <si>
+    <t>study design</t>
+  </si>
+  <si>
+    <t>data collection methods</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Applying Research Methods and Statistics (PSY)</t>
+  </si>
+  <si>
+    <t>Applying research methods and statistics </t>
+  </si>
+  <si>
+    <t>dr. J.E. Wassenberg-Severijnen</t>
+  </si>
+  <si>
+    <t>201800022, Faculty of Social Sciences</t>
+  </si>
+  <si>
+    <t>Applying research methods and statistics (PW &amp; OWW)</t>
+  </si>
+  <si>
+    <t>Applying research methods and statistics (ISS)</t>
+  </si>
+  <si>
+    <t>dr. J.E. Wassenberg-Severijnen,E.E. Vernooij</t>
+  </si>
+  <si>
+    <t>Applying research methods and statistics (SOC) </t>
+  </si>
+  <si>
+    <t>dr. J.E. Wassenberg-Severijnen, MSc. L. Mandemakers</t>
+  </si>
+  <si>
+    <t>prof. dr. H.J.A. Hoijtink</t>
+  </si>
+  <si>
+    <t>prof. dr. H.J.A. Hoijtink, dr. N.K. Schuurman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSBBSS03 and MSBBSS04 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1002,6 +1235,12 @@
       <name val="Open Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1029,7 +1268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1038,6 +1277,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1359,14 +1601,14 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="AN1" dT="2022-10-04T13:14:25.99" personId="{1C7E087E-E899-4ED6-827C-5BB62023D5BF}" id="{7912B0EA-387D-478B-95D3-9090A6112730}">
+  <threadedComment ref="AO1" dT="2022-10-04T13:14:25.99" personId="{1C7E087E-E899-4ED6-827C-5BB62023D5BF}" id="{7912B0EA-387D-478B-95D3-9090A6112730}">
     <text>INFOMUDR-evaluating probabilistic prediction models, such as discrimination and calibration, and how to asses them using cross-validation 
 INFOMEBD: developing and validating clinical prediction models using IPD</text>
   </threadedComment>
-  <threadedComment ref="AN26" dT="2022-10-07T17:19:06.74" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{235018C0-EEF6-44A5-9ED8-1B80DA82E322}">
+  <threadedComment ref="AO26" dT="2022-10-07T17:19:06.74" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{235018C0-EEF6-44A5-9ED8-1B80DA82E322}">
     <text>probability</text>
   </threadedComment>
-  <threadedComment ref="AT26" dT="2022-10-07T17:18:28.72" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{55636430-28F9-427E-8FC9-0523E795980C}">
+  <threadedComment ref="AU26" dT="2022-10-07T17:18:28.72" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{55636430-28F9-427E-8FC9-0523E795980C}">
     <text>concentration inequalities
 covariance matrices and Principle Component Analysis
 high-dimensional distributions
@@ -1379,7 +1621,7 @@
 deviations of random matrices
 sparse recovery</text>
   </threadedComment>
-  <threadedComment ref="AN30" dT="2022-10-08T17:30:06.70" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{4D3D460E-D00C-48E4-97F6-28235A8C037F}">
+  <threadedComment ref="AO30" dT="2022-10-08T17:30:06.70" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{4D3D460E-D00C-48E4-97F6-28235A8C037F}">
     <text>(Conditional) probability
 Inference
 Estimation
@@ -1390,25 +1632,59 @@
 Residuals
 Fitted values</text>
   </threadedComment>
-  <threadedComment ref="AN31" dT="2022-10-08T17:47:06.98" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{2C1CB73F-0B60-41E5-AECE-1427034B9CE3}">
+  <threadedComment ref="AO31" dT="2022-10-08T17:47:06.98" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{2C1CB73F-0B60-41E5-AECE-1427034B9CE3}">
     <text>using these data for estimation purposes</text>
   </threadedComment>
   <threadedComment ref="A35" dT="2022-10-08T18:10:51.15" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{35885A4E-3B89-4D6A-95CD-08862DFB9430}">
     <text>The course covers the essentials of qualitative research, in particular techniques for identifying themes, the making of systematic comparisons, and grounding interpretation in theory. Finally, it focuses on the principles of dovetailing primary ethnographic research, secondary data, and larger theoretical frames.</text>
   </threadedComment>
-  <threadedComment ref="AN49" dT="2022-10-11T10:33:57.67" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{0477E9A7-5E83-41B8-965E-BC68BE4572C4}">
+  <threadedComment ref="AO49" dT="2022-10-11T10:33:57.67" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{0477E9A7-5E83-41B8-965E-BC68BE4572C4}">
     <text>inference</text>
+  </threadedComment>
+  <threadedComment ref="A55" dT="2022-10-12T09:45:31.51" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{E2FFAAF8-7744-465F-9701-9A2AFF0D8FD2}">
+    <text>This course mentions in discription a statistical software use but I'm not sure what it is</text>
+  </threadedComment>
+  <threadedComment ref="AR62" dT="2022-10-12T15:01:51.51" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{971B0614-288D-4052-BBD0-23AC10C52401}">
+    <text>qualitative data</text>
+  </threadedComment>
+  <threadedComment ref="AU62" dT="2022-10-12T15:15:59.00" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{7C5818E2-1E6A-4677-95FD-D0E0F1BC44BF}">
+    <text>The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</text>
+  </threadedComment>
+  <threadedComment ref="A63" dT="2022-10-12T15:26:01.31" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{0F9D3427-B4EC-4231-A8B8-1CD7AE2C5236}">
+    <text>no course description</text>
+  </threadedComment>
+  <threadedComment ref="A63" dT="2022-10-12T15:26:28.06" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{F121CDAB-DC8B-48D6-9505-C2300F077CB9}" parentId="{0F9D3427-B4EC-4231-A8B8-1CD7AE2C5236}">
+    <text>only spss mantioned in the literature</text>
+  </threadedComment>
+  <threadedComment ref="AR64" dT="2022-10-12T15:29:32.58" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{B346AB8C-D5F8-4A60-B1CA-15714598AC1D}">
+    <text>qualitative data</text>
+  </threadedComment>
+  <threadedComment ref="AU64" dT="2022-10-12T15:29:11.55" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{FA9CD2C0-F5EE-473A-BF68-EE1E51FD7EED}">
+    <text>The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</text>
+  </threadedComment>
+  <threadedComment ref="AR65" dT="2022-10-12T15:33:36.58" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{74E5C956-2E55-47CF-908B-6DF2CA8BFF70}">
+    <text>qualitative data</text>
+  </threadedComment>
+  <threadedComment ref="AU65" dT="2022-10-12T15:33:22.60" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{D9A68AAD-F7F5-48E9-86BF-E791855CE074}">
+    <text>The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</text>
+  </threadedComment>
+  <threadedComment ref="AR66" dT="2022-10-12T15:36:24.67" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{D2CE96B7-DA8C-4491-9962-80A041D6783C}">
+    <text>The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</text>
+  </threadedComment>
+  <threadedComment ref="AU66" dT="2022-10-12T15:36:18.72" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{0156854D-B856-40C8-9F6A-56D1A73DF7D0}">
+    <text>The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{501E35CE-ACC9-4FC1-9D06-B7BA9C0949C0}">
-  <dimension ref="A1:BA53"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:BE67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH54" sqref="AH54"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BE67" sqref="BE67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1452,23 +1728,24 @@
     <col min="37" max="37" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="13" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="7" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="7" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="6.109375" customWidth="1"/>
+    <col min="41" max="41" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="7" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1509,7 +1786,7 @@
         <v>8</v>
       </c>
       <c r="N1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O1" t="s">
         <v>9</v>
@@ -1524,43 +1801,43 @@
         <v>11</v>
       </c>
       <c r="S1" t="s">
+        <v>277</v>
+      </c>
+      <c r="T1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1" t="s">
+        <v>293</v>
+      </c>
+      <c r="V1" t="s">
+        <v>88</v>
+      </c>
+      <c r="W1" t="s">
+        <v>109</v>
+      </c>
+      <c r="X1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y1" t="s">
         <v>111</v>
-      </c>
-      <c r="T1" t="s">
-        <v>65</v>
-      </c>
-      <c r="U1" t="s">
-        <v>90</v>
-      </c>
-      <c r="V1" t="s">
-        <v>89</v>
-      </c>
-      <c r="W1" t="s">
-        <v>112</v>
-      </c>
-      <c r="X1" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>114</v>
       </c>
       <c r="Z1" t="s">
         <v>31</v>
       </c>
       <c r="AA1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="AB1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AC1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AD1" t="s">
         <v>32</v>
       </c>
       <c r="AE1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="AF1" t="s">
         <v>33</v>
@@ -1572,64 +1849,76 @@
         <v>35</v>
       </c>
       <c r="AI1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>49</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>50</v>
       </c>
       <c r="AK1" t="s">
         <v>41</v>
       </c>
       <c r="AL1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AM1" t="s">
         <v>42</v>
       </c>
       <c r="AN1" t="s">
-        <v>43</v>
+        <v>261</v>
       </c>
       <c r="AO1" t="s">
-        <v>51</v>
+        <v>262</v>
       </c>
       <c r="AP1" t="s">
-        <v>169</v>
+        <v>50</v>
       </c>
       <c r="AQ1" t="s">
-        <v>83</v>
+        <v>166</v>
       </c>
       <c r="AR1" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="AS1" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="AT1" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="AU1" t="s">
-        <v>171</v>
+        <v>95</v>
       </c>
       <c r="AV1" t="s">
-        <v>115</v>
+        <v>168</v>
       </c>
       <c r="AW1" t="s">
-        <v>165</v>
+        <v>112</v>
       </c>
       <c r="AX1" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="AY1" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="AZ1" t="s">
-        <v>230</v>
+        <v>194</v>
       </c>
       <c r="BA1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>254</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>278</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>291</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1676,7 +1965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1744,7 +2033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1796,16 +2085,16 @@
       <c r="AM4">
         <v>1</v>
       </c>
-      <c r="AN4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AO4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
@@ -1817,10 +2106,10 @@
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I5">
         <v>7.5</v>
@@ -1849,16 +2138,16 @@
       <c r="AA5">
         <v>1</v>
       </c>
-      <c r="AN5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AO5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
@@ -1870,10 +2159,10 @@
         <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I6">
         <v>7.5</v>
@@ -1905,25 +2194,25 @@
       <c r="AJ6">
         <v>1</v>
       </c>
-      <c r="AN6">
-        <v>1</v>
-      </c>
       <c r="AO6">
         <v>1</v>
       </c>
-      <c r="AQ6">
+      <c r="AP6">
         <v>1</v>
       </c>
       <c r="AR6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AS6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
         <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
@@ -1935,10 +2224,10 @@
         <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I7">
         <v>7.5</v>
@@ -1967,19 +2256,19 @@
       <c r="AH7">
         <v>1</v>
       </c>
-      <c r="AN7">
-        <v>1</v>
-      </c>
-      <c r="AQ7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AO7">
+        <v>1</v>
+      </c>
+      <c r="AR7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
         <v>25</v>
@@ -1991,10 +2280,10 @@
         <v>26</v>
       </c>
       <c r="G8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" t="s">
         <v>61</v>
-      </c>
-      <c r="H8" t="s">
-        <v>62</v>
       </c>
       <c r="I8">
         <v>7.5</v>
@@ -2006,7 +2295,7 @@
         <v>2022</v>
       </c>
       <c r="L8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N8" t="s">
         <v>18</v>
@@ -2024,12 +2313,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
         <v>63</v>
-      </c>
-      <c r="B9" t="s">
-        <v>64</v>
       </c>
       <c r="D9" t="s">
         <v>25</v>
@@ -2041,10 +2330,10 @@
         <v>26</v>
       </c>
       <c r="G9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" t="s">
         <v>66</v>
-      </c>
-      <c r="H9" t="s">
-        <v>67</v>
       </c>
       <c r="I9">
         <v>7.5</v>
@@ -2070,16 +2359,16 @@
       <c r="T9">
         <v>1</v>
       </c>
-      <c r="AN9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AO9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
         <v>68</v>
-      </c>
-      <c r="B10" t="s">
-        <v>69</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
@@ -2091,10 +2380,10 @@
         <v>26</v>
       </c>
       <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s">
         <v>70</v>
-      </c>
-      <c r="H10" t="s">
-        <v>71</v>
       </c>
       <c r="I10">
         <v>7.5</v>
@@ -2124,12 +2413,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
@@ -2141,10 +2430,10 @@
         <v>26</v>
       </c>
       <c r="G11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I11">
         <v>7.5</v>
@@ -2170,16 +2459,16 @@
       <c r="S11">
         <v>1</v>
       </c>
-      <c r="AS11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AT11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
         <v>75</v>
-      </c>
-      <c r="B12" t="s">
-        <v>76</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
@@ -2191,10 +2480,10 @@
         <v>26</v>
       </c>
       <c r="G12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I12">
         <v>7.5</v>
@@ -2206,10 +2495,10 @@
         <v>2021</v>
       </c>
       <c r="L12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P12" t="s">
         <v>25</v>
@@ -2218,12 +2507,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
         <v>25</v>
@@ -2235,10 +2524,10 @@
         <v>26</v>
       </c>
       <c r="G13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I13">
         <v>7.5</v>
@@ -2267,31 +2556,31 @@
       <c r="AA13">
         <v>1</v>
       </c>
-      <c r="AQ13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AR13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D14">
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F14" t="s">
         <v>26</v>
       </c>
       <c r="G14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I14">
         <v>7.5</v>
@@ -2306,7 +2595,7 @@
         <v>4</v>
       </c>
       <c r="N14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q14">
         <v>1</v>
@@ -2330,12 +2619,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -2347,10 +2636,10 @@
         <v>26</v>
       </c>
       <c r="G15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I15">
         <v>7.5</v>
@@ -2365,10 +2654,10 @@
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="Q15">
         <v>1</v>
@@ -2382,34 +2671,34 @@
       <c r="AG15">
         <v>1</v>
       </c>
-      <c r="AQ15">
-        <v>1</v>
-      </c>
-      <c r="AT15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AR15">
+        <v>1</v>
+      </c>
+      <c r="AU15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F16" t="s">
         <v>26</v>
       </c>
       <c r="G16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I16">
         <v>7.5</v>
@@ -2424,14 +2713,14 @@
         <v>2</v>
       </c>
       <c r="M16" t="s">
+        <v>101</v>
+      </c>
+      <c r="N16" t="s">
+        <v>102</v>
+      </c>
+      <c r="P16" t="s">
         <v>103</v>
       </c>
-      <c r="N16" t="s">
-        <v>104</v>
-      </c>
-      <c r="P16" t="s">
-        <v>105</v>
-      </c>
       <c r="S16">
         <v>1</v>
       </c>
@@ -2447,16 +2736,16 @@
       <c r="Y16">
         <v>1</v>
       </c>
-      <c r="AQ16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AR16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
@@ -2468,10 +2757,10 @@
         <v>26</v>
       </c>
       <c r="G17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I17">
         <v>7.5</v>
@@ -2486,7 +2775,7 @@
         <v>4</v>
       </c>
       <c r="N17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P17" t="s">
         <v>25</v>
@@ -2494,22 +2783,22 @@
       <c r="Q17">
         <v>1</v>
       </c>
-      <c r="AT17">
-        <v>1</v>
-      </c>
       <c r="AU17">
         <v>1</v>
       </c>
       <c r="AV17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AW17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D18" t="s">
         <v>25</v>
@@ -2521,10 +2810,10 @@
         <v>26</v>
       </c>
       <c r="G18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I18">
         <v>7.5</v>
@@ -2539,7 +2828,7 @@
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="P18" t="s">
         <v>25</v>
@@ -2553,31 +2842,31 @@
       <c r="AE18">
         <v>1</v>
       </c>
-      <c r="AT18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AU18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F19" t="s">
         <v>26</v>
       </c>
       <c r="G19" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H19" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I19">
         <v>7.5</v>
@@ -2592,42 +2881,42 @@
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="P19" t="s">
+        <v>124</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="X19">
+        <v>1</v>
+      </c>
+      <c r="AF19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>127</v>
       </c>
-      <c r="V19">
-        <v>1</v>
-      </c>
-      <c r="X19">
-        <v>1</v>
-      </c>
-      <c r="AF19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>130</v>
-      </c>
       <c r="B20" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F20" t="s">
         <v>26</v>
       </c>
       <c r="G20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I20">
         <v>7.5</v>
@@ -2642,33 +2931,33 @@
         <v>3</v>
       </c>
       <c r="M20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N20" t="s">
+        <v>125</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21" t="s">
         <v>128</v>
-      </c>
-      <c r="S20">
-        <v>1</v>
-      </c>
-      <c r="W20">
-        <v>1</v>
-      </c>
-      <c r="X20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>132</v>
-      </c>
-      <c r="B21" t="s">
-        <v>131</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F21" t="s">
         <v>26</v>
@@ -2686,42 +2975,42 @@
         <v>3</v>
       </c>
       <c r="N21" t="s">
+        <v>130</v>
+      </c>
+      <c r="P21" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="Z21">
+        <v>1</v>
+      </c>
+      <c r="AD21">
+        <v>1</v>
+      </c>
+      <c r="AE21">
+        <v>1</v>
+      </c>
+      <c r="AG21">
+        <v>1</v>
+      </c>
+      <c r="AR21">
+        <v>1</v>
+      </c>
+      <c r="AW21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" t="s">
         <v>133</v>
-      </c>
-      <c r="P21" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-      <c r="S21">
-        <v>1</v>
-      </c>
-      <c r="Z21">
-        <v>1</v>
-      </c>
-      <c r="AD21">
-        <v>1</v>
-      </c>
-      <c r="AE21">
-        <v>1</v>
-      </c>
-      <c r="AG21">
-        <v>1</v>
-      </c>
-      <c r="AQ21">
-        <v>1</v>
-      </c>
-      <c r="AV21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>135</v>
-      </c>
-      <c r="B22" t="s">
-        <v>136</v>
       </c>
       <c r="D22" t="s">
         <v>25</v>
@@ -2733,10 +3022,10 @@
         <v>26</v>
       </c>
       <c r="G22" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H22" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I22">
         <v>7.5</v>
@@ -2751,7 +3040,7 @@
         <v>1</v>
       </c>
       <c r="M22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="S22">
         <v>1</v>
@@ -2762,31 +3051,31 @@
       <c r="AG22">
         <v>1</v>
       </c>
-      <c r="AU22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AV22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D23">
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F23" t="s">
         <v>26</v>
       </c>
       <c r="G23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I23">
         <v>7.5</v>
@@ -2801,10 +3090,10 @@
         <v>4</v>
       </c>
       <c r="M23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N23" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="S23">
         <v>1</v>
@@ -2815,16 +3104,16 @@
       <c r="AA23">
         <v>1</v>
       </c>
-      <c r="AQ23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AR23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B24" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D24" t="s">
         <v>25</v>
@@ -2836,10 +3125,10 @@
         <v>26</v>
       </c>
       <c r="G24" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I24">
         <v>7.5</v>
@@ -2856,31 +3145,31 @@
       <c r="AE24">
         <v>1</v>
       </c>
-      <c r="AV24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AW24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B25" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F25" t="s">
         <v>26</v>
       </c>
       <c r="G25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H25" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I25">
         <v>7.5</v>
@@ -2895,10 +3184,10 @@
         <v>1</v>
       </c>
       <c r="N25" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="AA25">
         <v>1</v>
@@ -2906,19 +3195,19 @@
       <c r="AE25">
         <v>1</v>
       </c>
-      <c r="AT25">
-        <v>1</v>
-      </c>
-      <c r="AW25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AU25">
+        <v>1</v>
+      </c>
+      <c r="AX25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B26" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D26" t="s">
         <v>25</v>
@@ -2930,10 +3219,10 @@
         <v>26</v>
       </c>
       <c r="G26" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H26" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I26">
         <v>7.5</v>
@@ -2942,7 +3231,7 @@
         <v>2021</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="P26" t="s">
         <v>26</v>
@@ -2950,22 +3239,22 @@
       <c r="Q26">
         <v>1</v>
       </c>
-      <c r="AN26">
-        <v>1</v>
-      </c>
-      <c r="AP26">
-        <v>1</v>
-      </c>
-      <c r="AT26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AO26">
+        <v>1</v>
+      </c>
+      <c r="AQ26">
+        <v>1</v>
+      </c>
+      <c r="AU26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D27" t="s">
         <v>25</v>
@@ -2977,10 +3266,10 @@
         <v>26</v>
       </c>
       <c r="G27" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H27" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I27">
         <v>3</v>
@@ -2992,10 +3281,10 @@
         <v>2022</v>
       </c>
       <c r="L27" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="N27" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="Q27">
         <v>1</v>
@@ -3013,12 +3302,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B28" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D28" t="s">
         <v>25</v>
@@ -3033,7 +3322,7 @@
         <v>19</v>
       </c>
       <c r="H28" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I28">
         <v>7.5</v>
@@ -3048,7 +3337,7 @@
         <v>2</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="P28" t="s">
         <v>25</v>
@@ -3068,13 +3357,13 @@
       <c r="AF28">
         <v>1</v>
       </c>
-      <c r="AW28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AX28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B29">
         <v>201900027</v>
@@ -3086,13 +3375,13 @@
         <v>17</v>
       </c>
       <c r="F29" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G29" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H29" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I29">
         <v>7.5</v>
@@ -3107,7 +3396,7 @@
         <v>4</v>
       </c>
       <c r="M29" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="Q29">
         <v>1</v>
@@ -3124,25 +3413,25 @@
       <c r="AK29">
         <v>1</v>
       </c>
-      <c r="AN29">
-        <v>1</v>
-      </c>
-      <c r="AP29">
-        <v>1</v>
-      </c>
-      <c r="AT29">
-        <v>1</v>
-      </c>
-      <c r="AV29">
-        <v>1</v>
-      </c>
-      <c r="AX29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AO29">
+        <v>1</v>
+      </c>
+      <c r="AQ29">
+        <v>1</v>
+      </c>
+      <c r="AU29">
+        <v>1</v>
+      </c>
+      <c r="AW29">
+        <v>1</v>
+      </c>
+      <c r="AY29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B30">
         <v>201900026</v>
@@ -3154,13 +3443,13 @@
         <v>17</v>
       </c>
       <c r="F30" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G30" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H30" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I30">
         <v>7.5</v>
@@ -3175,7 +3464,7 @@
         <v>2</v>
       </c>
       <c r="M30" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="Q30">
         <v>1</v>
@@ -3192,19 +3481,19 @@
       <c r="AL30">
         <v>1</v>
       </c>
-      <c r="AN30">
-        <v>1</v>
-      </c>
-      <c r="AV30">
-        <v>1</v>
-      </c>
-      <c r="AX30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AO30">
+        <v>1</v>
+      </c>
+      <c r="AW30">
+        <v>1</v>
+      </c>
+      <c r="AY30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B31">
         <v>201700013</v>
@@ -3216,13 +3505,13 @@
         <v>17</v>
       </c>
       <c r="F31" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G31" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H31" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I31">
         <v>2</v>
@@ -3237,36 +3526,36 @@
         <v>1</v>
       </c>
       <c r="M31" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="P31" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="AE31">
+        <v>1</v>
+      </c>
+      <c r="AK31">
+        <v>1</v>
+      </c>
+      <c r="AO31">
+        <v>1</v>
+      </c>
+      <c r="AY31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>181</v>
-      </c>
-      <c r="Q31">
-        <v>1</v>
-      </c>
-      <c r="S31">
-        <v>1</v>
-      </c>
-      <c r="U31">
-        <v>1</v>
-      </c>
-      <c r="AE31">
-        <v>1</v>
-      </c>
-      <c r="AK31">
-        <v>1</v>
-      </c>
-      <c r="AN31">
-        <v>1</v>
-      </c>
-      <c r="AX31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>184</v>
       </c>
       <c r="B32">
         <v>201600038</v>
@@ -3278,10 +3567,10 @@
         <v>17</v>
       </c>
       <c r="F32" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G32" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I32">
         <v>7.5</v>
@@ -3293,12 +3582,12 @@
         <v>2020</v>
       </c>
       <c r="L32" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="33" spans="1:52" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B33">
         <v>200700054</v>
@@ -3307,13 +3596,13 @@
         <v>3</v>
       </c>
       <c r="E33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F33" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G33" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I33">
         <v>7.5</v>
@@ -3325,9 +3614,9 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="34" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B34">
         <v>202200015</v>
@@ -3339,10 +3628,10 @@
         <v>17</v>
       </c>
       <c r="F34" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G34" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I34">
         <v>2</v>
@@ -3351,13 +3640,13 @@
         <v>2022</v>
       </c>
       <c r="L34" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="N34">
         <v>1</v>
       </c>
       <c r="P34" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="Q34">
         <v>1</v>
@@ -3369,9 +3658,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:52" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B35">
         <v>201000091</v>
@@ -3383,13 +3672,13 @@
         <v>17</v>
       </c>
       <c r="F35" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G35" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H35" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I35">
         <v>7.5</v>
@@ -3401,18 +3690,18 @@
         <v>2022</v>
       </c>
       <c r="L35" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M35" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="P35">
         <v>201100072</v>
       </c>
     </row>
-    <row r="36" spans="1:52" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B36">
         <v>201800138</v>
@@ -3424,13 +3713,13 @@
         <v>17</v>
       </c>
       <c r="F36" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G36" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H36" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I36">
         <v>7.5</v>
@@ -3445,10 +3734,10 @@
         <v>2</v>
       </c>
       <c r="M36" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="P36">
         <v>200300022</v>
@@ -3456,25 +3745,25 @@
       <c r="Q36">
         <v>1</v>
       </c>
-      <c r="AN36">
-        <v>1</v>
-      </c>
-      <c r="AQ36">
-        <v>1</v>
-      </c>
-      <c r="AY36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AO36">
+        <v>1</v>
+      </c>
+      <c r="AR36">
+        <v>1</v>
+      </c>
+      <c r="AZ36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B37">
         <v>201800139</v>
       </c>
       <c r="C37" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D37">
         <v>3</v>
@@ -3483,7 +3772,7 @@
         <v>17</v>
       </c>
       <c r="F37" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I37">
         <v>5</v>
@@ -3498,9 +3787,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B38">
         <v>201500130</v>
@@ -3512,10 +3801,10 @@
         <v>17</v>
       </c>
       <c r="F38" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G38" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="I38">
         <v>7.5</v>
@@ -3530,30 +3819,30 @@
         <v>3</v>
       </c>
       <c r="N38" t="s">
+        <v>199</v>
+      </c>
+      <c r="P38" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
+      </c>
+      <c r="T38">
+        <v>1</v>
+      </c>
+      <c r="Y38">
+        <v>1</v>
+      </c>
+      <c r="AE38">
+        <v>1</v>
+      </c>
+      <c r="AK38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>202</v>
-      </c>
-      <c r="P38" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q38">
-        <v>1</v>
-      </c>
-      <c r="T38">
-        <v>1</v>
-      </c>
-      <c r="Y38">
-        <v>1</v>
-      </c>
-      <c r="AE38">
-        <v>1</v>
-      </c>
-      <c r="AK38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>205</v>
       </c>
       <c r="B39">
         <v>200300022</v>
@@ -3562,16 +3851,16 @@
         <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F39" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G39" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H39" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I39">
         <v>7.5</v>
@@ -3586,24 +3875,24 @@
         <v>2</v>
       </c>
       <c r="N39" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="P39" t="s">
+        <v>204</v>
+      </c>
+      <c r="AO39">
+        <v>1</v>
+      </c>
+      <c r="AR39">
+        <v>1</v>
+      </c>
+      <c r="AZ39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>207</v>
-      </c>
-      <c r="AN39">
-        <v>1</v>
-      </c>
-      <c r="AQ39">
-        <v>1</v>
-      </c>
-      <c r="AY39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>210</v>
       </c>
       <c r="B40">
         <v>201300001</v>
@@ -3615,7 +3904,7 @@
         <v>17</v>
       </c>
       <c r="F40" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I40">
         <v>7.5</v>
@@ -3627,13 +3916,13 @@
         <v>2022</v>
       </c>
       <c r="L40" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="M40" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="P40" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="U40">
         <v>1</v>
@@ -3650,19 +3939,19 @@
       <c r="AK40">
         <v>1</v>
       </c>
-      <c r="AN40">
-        <v>1</v>
-      </c>
-      <c r="AP40">
+      <c r="AO40">
         <v>1</v>
       </c>
       <c r="AQ40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AR40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B41">
         <v>202100022</v>
@@ -3671,12 +3960,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B42" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D42" t="s">
         <v>25</v>
@@ -3688,10 +3977,10 @@
         <v>26</v>
       </c>
       <c r="G42" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="H42" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I42">
         <v>7.5</v>
@@ -3706,7 +3995,7 @@
         <v>1</v>
       </c>
       <c r="M42" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="P42" t="s">
         <v>25</v>
@@ -3726,28 +4015,28 @@
       <c r="AL42">
         <v>1</v>
       </c>
-      <c r="AN42">
-        <v>1</v>
-      </c>
-      <c r="AP42">
-        <v>1</v>
-      </c>
-      <c r="AT42">
-        <v>1</v>
-      </c>
-      <c r="AV42">
-        <v>1</v>
-      </c>
-      <c r="AX42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AO42">
+        <v>1</v>
+      </c>
+      <c r="AQ42">
+        <v>1</v>
+      </c>
+      <c r="AU42">
+        <v>1</v>
+      </c>
+      <c r="AW42">
+        <v>1</v>
+      </c>
+      <c r="AY42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B43" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D43" t="s">
         <v>25</v>
@@ -3759,10 +4048,10 @@
         <v>26</v>
       </c>
       <c r="G43" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H43" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I43">
         <v>7.5</v>
@@ -3777,7 +4066,7 @@
         <v>2</v>
       </c>
       <c r="M43" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="P43" t="s">
         <v>25</v>
@@ -3806,25 +4095,25 @@
       <c r="AK43">
         <v>1</v>
       </c>
-      <c r="AN43">
-        <v>1</v>
-      </c>
-      <c r="AT43">
-        <v>1</v>
-      </c>
-      <c r="AV43">
-        <v>1</v>
-      </c>
-      <c r="AX43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AO43">
+        <v>1</v>
+      </c>
+      <c r="AU43">
+        <v>1</v>
+      </c>
+      <c r="AW43">
+        <v>1</v>
+      </c>
+      <c r="AY43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D44" t="s">
         <v>25</v>
@@ -3833,10 +4122,10 @@
         <v>17</v>
       </c>
       <c r="F44" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G44" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="I44">
         <v>1.5</v>
@@ -3845,7 +4134,7 @@
         <v>2022</v>
       </c>
       <c r="R44" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="AC44">
         <v>1</v>
@@ -3860,12 +4149,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B45" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D45">
         <v>3</v>
@@ -3874,13 +4163,13 @@
         <v>17</v>
       </c>
       <c r="F45" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G45" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H45" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="I45">
         <v>1.5</v>
@@ -3889,7 +4178,7 @@
         <v>2022</v>
       </c>
       <c r="R45" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="AE45">
         <v>1</v>
@@ -3897,16 +4186,16 @@
       <c r="AG45">
         <v>1</v>
       </c>
-      <c r="AX45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AY45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B46" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D46">
         <v>3</v>
@@ -3918,10 +4207,10 @@
         <v>26</v>
       </c>
       <c r="G46" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H46" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="I46">
         <v>1.5</v>
@@ -3930,24 +4219,24 @@
         <v>2022</v>
       </c>
       <c r="R46" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="AE46">
         <v>1</v>
       </c>
-      <c r="AX46">
-        <v>1</v>
-      </c>
-      <c r="AZ46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AY46">
+        <v>1</v>
+      </c>
+      <c r="BA46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D47" t="s">
         <v>25</v>
@@ -3956,13 +4245,13 @@
         <v>17</v>
       </c>
       <c r="F47" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G47" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H47" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="I47">
         <v>1.5</v>
@@ -3974,7 +4263,7 @@
         <v>60</v>
       </c>
       <c r="R47" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="Z47">
         <v>1</v>
@@ -3988,28 +4277,28 @@
       <c r="AK47">
         <v>1</v>
       </c>
-      <c r="AN47">
-        <v>1</v>
-      </c>
-      <c r="AP47">
-        <v>1</v>
-      </c>
-      <c r="AT47">
-        <v>1</v>
-      </c>
-      <c r="AV47">
-        <v>1</v>
-      </c>
-      <c r="AX47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AO47">
+        <v>1</v>
+      </c>
+      <c r="AQ47">
+        <v>1</v>
+      </c>
+      <c r="AU47">
+        <v>1</v>
+      </c>
+      <c r="AW47">
+        <v>1</v>
+      </c>
+      <c r="AY47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B48" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D48" t="s">
         <v>25</v>
@@ -4018,13 +4307,13 @@
         <v>17</v>
       </c>
       <c r="F48" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G48" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H48" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I48">
         <v>1.5</v>
@@ -4036,7 +4325,7 @@
         <v>80</v>
       </c>
       <c r="R48" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="Z48">
         <v>1</v>
@@ -4053,25 +4342,28 @@
       <c r="AG48">
         <v>1</v>
       </c>
-      <c r="AN48">
-        <v>1</v>
-      </c>
-      <c r="AQ48">
-        <v>1</v>
-      </c>
-      <c r="AT48">
-        <v>1</v>
-      </c>
-      <c r="AX48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AO48">
+        <v>1</v>
+      </c>
+      <c r="AR48">
+        <v>1</v>
+      </c>
+      <c r="AU48">
+        <v>1</v>
+      </c>
+      <c r="AY48">
+        <v>1</v>
+      </c>
+      <c r="BD48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B49" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D49" t="s">
         <v>25</v>
@@ -4080,13 +4372,13 @@
         <v>17</v>
       </c>
       <c r="F49" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G49" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H49" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="I49">
         <v>1.5</v>
@@ -4098,7 +4390,7 @@
         <v>50</v>
       </c>
       <c r="R49" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="Y49">
         <v>1</v>
@@ -4109,25 +4401,25 @@
       <c r="AK49">
         <v>1</v>
       </c>
-      <c r="AN49">
-        <v>1</v>
-      </c>
-      <c r="AQ49">
-        <v>1</v>
-      </c>
-      <c r="AV49">
-        <v>1</v>
-      </c>
-      <c r="AX49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AO49">
+        <v>1</v>
+      </c>
+      <c r="AR49">
+        <v>1</v>
+      </c>
+      <c r="AW49">
+        <v>1</v>
+      </c>
+      <c r="AY49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B50" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D50" t="s">
         <v>25</v>
@@ -4136,13 +4428,13 @@
         <v>17</v>
       </c>
       <c r="F50" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G50" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H50" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="I50">
         <v>1.5</v>
@@ -4154,7 +4446,7 @@
         <v>80</v>
       </c>
       <c r="R50" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AE50">
         <v>1</v>
@@ -4162,22 +4454,22 @@
       <c r="AK50">
         <v>1</v>
       </c>
-      <c r="AN50">
-        <v>1</v>
-      </c>
-      <c r="AR50">
-        <v>1</v>
-      </c>
-      <c r="AV50">
-        <v>1</v>
-      </c>
-      <c r="AX50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AO50">
+        <v>1</v>
+      </c>
+      <c r="AS50">
+        <v>1</v>
+      </c>
+      <c r="AW50">
+        <v>1</v>
+      </c>
+      <c r="AY50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B51">
         <v>202100012</v>
@@ -4189,13 +4481,13 @@
         <v>17</v>
       </c>
       <c r="F51" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G51" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H51" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="I51">
         <v>7.5</v>
@@ -4210,24 +4502,24 @@
         <v>4</v>
       </c>
       <c r="N51" t="s">
+        <v>249</v>
+      </c>
+      <c r="P51" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q51">
+        <v>1</v>
+      </c>
+      <c r="S51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>251</v>
+      </c>
+      <c r="B52" t="s">
         <v>252</v>
-      </c>
-      <c r="P51" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q51">
-        <v>1</v>
-      </c>
-      <c r="S51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>254</v>
-      </c>
-      <c r="B52" t="s">
-        <v>255</v>
       </c>
       <c r="D52" t="s">
         <v>25</v>
@@ -4239,10 +4531,10 @@
         <v>26</v>
       </c>
       <c r="G52" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H52" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="I52">
         <v>7.5</v>
@@ -4257,7 +4549,7 @@
         <v>4</v>
       </c>
       <c r="N52" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P52" t="s">
         <v>25</v>
@@ -4265,20 +4557,750 @@
       <c r="Q52">
         <v>1</v>
       </c>
-      <c r="BA52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="BB52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:57" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>255</v>
+      </c>
+      <c r="B53" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="54" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>257</v>
+      </c>
+      <c r="B54">
+        <v>201900025</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>84</v>
+      </c>
+      <c r="F54" t="s">
+        <v>171</v>
+      </c>
+      <c r="G54" t="s">
         <v>258</v>
       </c>
-      <c r="B53" t="s">
+      <c r="H54" t="s">
+        <v>258</v>
+      </c>
+      <c r="I54">
+        <v>7.5</v>
+      </c>
+      <c r="J54" t="s">
         <v>259</v>
       </c>
+      <c r="K54">
+        <v>2022</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
+      <c r="N54" t="s">
+        <v>170</v>
+      </c>
+      <c r="P54" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q54">
+        <v>1</v>
+      </c>
+      <c r="S54">
+        <v>1</v>
+      </c>
+      <c r="AO54">
+        <v>1</v>
+      </c>
+      <c r="AV54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>263</v>
+      </c>
+      <c r="B55">
+        <v>202200104</v>
+      </c>
+      <c r="D55">
+        <v>3</v>
+      </c>
+      <c r="E55" t="s">
+        <v>17</v>
+      </c>
+      <c r="F55" t="s">
+        <v>171</v>
+      </c>
+      <c r="G55" t="s">
+        <v>264</v>
+      </c>
+      <c r="H55" t="s">
+        <v>265</v>
+      </c>
+      <c r="I55">
+        <v>7.5</v>
+      </c>
+      <c r="J55" t="s">
+        <v>259</v>
+      </c>
+      <c r="K55">
+        <v>2022</v>
+      </c>
+      <c r="L55">
+        <v>2</v>
+      </c>
+      <c r="P55" t="s">
+        <v>266</v>
+      </c>
+      <c r="S55">
+        <v>1</v>
+      </c>
+      <c r="AN55">
+        <v>1</v>
+      </c>
+      <c r="AO55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>267</v>
+      </c>
+      <c r="B56">
+        <v>201800032</v>
+      </c>
+      <c r="C56" t="s">
+        <v>268</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56" t="s">
+        <v>17</v>
+      </c>
+      <c r="F56" t="s">
+        <v>171</v>
+      </c>
+      <c r="G56" t="s">
+        <v>269</v>
+      </c>
+      <c r="H56" t="s">
+        <v>271</v>
+      </c>
+      <c r="I56">
+        <v>5</v>
+      </c>
+      <c r="J56" t="s">
+        <v>259</v>
+      </c>
+      <c r="K56">
+        <v>2022</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
+      </c>
+      <c r="S56">
+        <v>1</v>
+      </c>
+      <c r="AO56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>270</v>
+      </c>
+      <c r="B57">
+        <v>200300009</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57" t="s">
+        <v>17</v>
+      </c>
+      <c r="F57" t="s">
+        <v>171</v>
+      </c>
+      <c r="G57" t="s">
+        <v>269</v>
+      </c>
+      <c r="H57" t="s">
+        <v>272</v>
+      </c>
+      <c r="I57">
+        <v>7.5</v>
+      </c>
+      <c r="J57" t="s">
+        <v>259</v>
+      </c>
+      <c r="K57">
+        <v>2022</v>
+      </c>
+      <c r="L57">
+        <v>1</v>
+      </c>
+      <c r="N57" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q57">
+        <v>1</v>
+      </c>
+      <c r="S57">
+        <v>1</v>
+      </c>
+      <c r="AO57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>274</v>
+      </c>
+      <c r="B58">
+        <v>200600027</v>
+      </c>
+      <c r="D58" t="s">
+        <v>25</v>
+      </c>
+      <c r="E58" t="s">
+        <v>17</v>
+      </c>
+      <c r="F58" t="s">
+        <v>171</v>
+      </c>
+      <c r="G58" t="s">
+        <v>275</v>
+      </c>
+      <c r="H58" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="I58">
+        <v>7.5</v>
+      </c>
+      <c r="J58" t="s">
+        <v>259</v>
+      </c>
+      <c r="K58">
+        <v>2022</v>
+      </c>
+      <c r="L58" t="s">
+        <v>187</v>
+      </c>
+      <c r="M58" t="s">
+        <v>276</v>
+      </c>
+      <c r="P58" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q58">
+        <v>1</v>
+      </c>
+      <c r="S58">
+        <v>1</v>
+      </c>
+      <c r="AO58">
+        <v>1</v>
+      </c>
+      <c r="AY58">
+        <v>1</v>
+      </c>
+      <c r="AZ58">
+        <v>1</v>
+      </c>
+      <c r="BC58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>279</v>
+      </c>
+      <c r="B59">
+        <v>201900054</v>
+      </c>
+      <c r="D59">
+        <v>3</v>
+      </c>
+      <c r="E59" t="s">
+        <v>84</v>
+      </c>
+      <c r="F59" t="s">
+        <v>171</v>
+      </c>
+      <c r="G59" t="s">
+        <v>281</v>
+      </c>
+      <c r="H59" t="s">
+        <v>280</v>
+      </c>
+      <c r="I59">
+        <v>7.5</v>
+      </c>
+      <c r="J59" t="s">
+        <v>259</v>
+      </c>
+      <c r="K59">
+        <v>2022</v>
+      </c>
+      <c r="L59">
+        <v>2</v>
+      </c>
+      <c r="N59" t="s">
+        <v>283</v>
+      </c>
+      <c r="P59" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q59">
+        <v>1</v>
+      </c>
+      <c r="S59">
+        <v>1</v>
+      </c>
+      <c r="AO59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>284</v>
+      </c>
+      <c r="B60">
+        <v>201900398</v>
+      </c>
+      <c r="D60">
+        <v>3</v>
+      </c>
+      <c r="E60" t="s">
+        <v>84</v>
+      </c>
+      <c r="F60" t="s">
+        <v>171</v>
+      </c>
+      <c r="G60" t="s">
+        <v>285</v>
+      </c>
+      <c r="I60">
+        <v>7.5</v>
+      </c>
+      <c r="J60" t="s">
+        <v>259</v>
+      </c>
+      <c r="K60">
+        <v>2022</v>
+      </c>
+      <c r="L60">
+        <v>2</v>
+      </c>
+      <c r="P60" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q60">
+        <v>1</v>
+      </c>
+      <c r="S60">
+        <v>1</v>
+      </c>
+      <c r="AO60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>287</v>
+      </c>
+      <c r="B61">
+        <v>200600023</v>
+      </c>
+      <c r="D61" t="s">
+        <v>25</v>
+      </c>
+      <c r="E61" t="s">
+        <v>17</v>
+      </c>
+      <c r="F61" t="s">
+        <v>171</v>
+      </c>
+      <c r="G61" t="s">
+        <v>288</v>
+      </c>
+      <c r="H61" t="s">
+        <v>290</v>
+      </c>
+      <c r="I61">
+        <v>7.5</v>
+      </c>
+      <c r="J61" t="s">
+        <v>259</v>
+      </c>
+      <c r="K61">
+        <v>2022</v>
+      </c>
+      <c r="L61" t="s">
+        <v>154</v>
+      </c>
+      <c r="M61" t="s">
+        <v>276</v>
+      </c>
+      <c r="P61" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q61">
+        <v>1</v>
+      </c>
+      <c r="S61">
+        <v>1</v>
+      </c>
+      <c r="AO61">
+        <v>1</v>
+      </c>
+      <c r="AY61">
+        <v>1</v>
+      </c>
+      <c r="AZ61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>295</v>
+      </c>
+      <c r="B62">
+        <v>201800055</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62" t="s">
+        <v>84</v>
+      </c>
+      <c r="F62" t="s">
+        <v>171</v>
+      </c>
+      <c r="G62" t="s">
+        <v>280</v>
+      </c>
+      <c r="H62" t="s">
+        <v>294</v>
+      </c>
+      <c r="I62">
+        <v>7.5</v>
+      </c>
+      <c r="J62" t="s">
+        <v>259</v>
+      </c>
+      <c r="K62">
+        <v>2022</v>
+      </c>
+      <c r="L62">
+        <v>3</v>
+      </c>
+      <c r="P62" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q62">
+        <v>1</v>
+      </c>
+      <c r="S62">
+        <v>1</v>
+      </c>
+      <c r="U62">
+        <v>1</v>
+      </c>
+      <c r="AR62">
+        <v>1</v>
+      </c>
+      <c r="AU62">
+        <v>1</v>
+      </c>
+      <c r="BE62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>296</v>
+      </c>
+      <c r="B63">
+        <v>201800028</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63" t="s">
+        <v>84</v>
+      </c>
+      <c r="F63" t="s">
+        <v>171</v>
+      </c>
+      <c r="G63" t="s">
+        <v>297</v>
+      </c>
+      <c r="H63" t="s">
+        <v>297</v>
+      </c>
+      <c r="I63">
+        <v>7.5</v>
+      </c>
+      <c r="J63" t="s">
+        <v>259</v>
+      </c>
+      <c r="K63">
+        <v>2022</v>
+      </c>
+      <c r="L63">
+        <v>3</v>
+      </c>
+      <c r="P63" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="64" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>299</v>
+      </c>
+      <c r="B64">
+        <v>201800173</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s">
+        <v>84</v>
+      </c>
+      <c r="F64" t="s">
+        <v>171</v>
+      </c>
+      <c r="G64" t="s">
+        <v>297</v>
+      </c>
+      <c r="I64">
+        <v>7.5</v>
+      </c>
+      <c r="J64" t="s">
+        <v>259</v>
+      </c>
+      <c r="K64">
+        <v>2022</v>
+      </c>
+      <c r="L64">
+        <v>4</v>
+      </c>
+      <c r="P64">
+        <v>201800171</v>
+      </c>
+      <c r="S64">
+        <v>1</v>
+      </c>
+      <c r="U64">
+        <v>1</v>
+      </c>
+      <c r="AR64">
+        <v>1</v>
+      </c>
+      <c r="AU64">
+        <v>1</v>
+      </c>
+      <c r="BE64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>300</v>
+      </c>
+      <c r="B65">
+        <v>201800025</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s">
+        <v>84</v>
+      </c>
+      <c r="F65" t="s">
+        <v>171</v>
+      </c>
+      <c r="G65" t="s">
+        <v>297</v>
+      </c>
+      <c r="H65" t="s">
+        <v>301</v>
+      </c>
+      <c r="I65">
+        <v>7.5</v>
+      </c>
+      <c r="J65" t="s">
+        <v>259</v>
+      </c>
+      <c r="K65">
+        <v>2022</v>
+      </c>
+      <c r="L65">
+        <v>3</v>
+      </c>
+      <c r="N65" t="s">
+        <v>282</v>
+      </c>
+      <c r="P65">
+        <v>201800022</v>
+      </c>
+      <c r="Q65">
+        <v>1</v>
+      </c>
+      <c r="S65">
+        <v>1</v>
+      </c>
+      <c r="U65">
+        <v>1</v>
+      </c>
+      <c r="AR65">
+        <v>1</v>
+      </c>
+      <c r="AU65">
+        <v>1</v>
+      </c>
+      <c r="BE65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>302</v>
+      </c>
+      <c r="B66">
+        <v>201800024</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="E66" t="s">
+        <v>84</v>
+      </c>
+      <c r="F66" t="s">
+        <v>171</v>
+      </c>
+      <c r="G66" t="s">
+        <v>297</v>
+      </c>
+      <c r="H66" t="s">
+        <v>303</v>
+      </c>
+      <c r="I66">
+        <v>7.5</v>
+      </c>
+      <c r="J66" t="s">
+        <v>259</v>
+      </c>
+      <c r="K66">
+        <v>2022</v>
+      </c>
+      <c r="L66">
+        <v>3</v>
+      </c>
+      <c r="P66">
+        <v>201800022</v>
+      </c>
+      <c r="Q66">
+        <v>1</v>
+      </c>
+      <c r="S66">
+        <v>1</v>
+      </c>
+      <c r="U66">
+        <v>1</v>
+      </c>
+      <c r="AR66">
+        <v>1</v>
+      </c>
+      <c r="AU66">
+        <v>1</v>
+      </c>
+      <c r="BE66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>261</v>
+      </c>
+      <c r="B67">
+        <v>201300007</v>
+      </c>
+      <c r="D67" t="s">
+        <v>25</v>
+      </c>
+      <c r="E67" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" t="s">
+        <v>171</v>
+      </c>
+      <c r="G67" t="s">
+        <v>304</v>
+      </c>
+      <c r="H67" t="s">
+        <v>305</v>
+      </c>
+      <c r="I67">
+        <v>7.5</v>
+      </c>
+      <c r="J67" t="s">
+        <v>259</v>
+      </c>
+      <c r="K67">
+        <v>2022</v>
+      </c>
+      <c r="L67" t="s">
+        <v>154</v>
+      </c>
+      <c r="M67" t="s">
+        <v>208</v>
+      </c>
+      <c r="P67" t="s">
+        <v>306</v>
+      </c>
+      <c r="S67">
+        <v>1</v>
+      </c>
+      <c r="AE67">
+        <v>1</v>
+      </c>
+      <c r="AK67">
+        <v>1</v>
+      </c>
+      <c r="AL67">
+        <v>1</v>
+      </c>
+      <c r="AN67">
+        <v>1</v>
+      </c>
+      <c r="AO67">
+        <v>1</v>
+      </c>
+      <c r="AW67">
+        <v>1</v>
+      </c>
+      <c r="AY67">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AY53" xr:uid="{501E35CE-ACC9-4FC1-9D06-B7BA9C0949C0}"/>
+  <autoFilter ref="A1:AZ53" xr:uid="{501E35CE-ACC9-4FC1-9D06-B7BA9C0949C0}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Faculty of Social Sciences"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4287,21 +5309,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003B9512465F22C14FB160D435DD2FE48B" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dcc4c4d2e32b8c8f0f92638a638e9a27">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a49ec6c6-c19a-430d-9e65-9140718fcb4c" xmlns:ns4="11ce1b15-5995-4f89-8454-542f1e930605" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b0d976c7959d1c14d6037bfd1f975a8" ns3:_="" ns4:_="">
     <xsd:import namespace="a49ec6c6-c19a-430d-9e65-9140718fcb4c"/>
@@ -4530,32 +5537,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{258C3525-B843-4DF1-AAB7-9A7C9FE670BA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a49ec6c6-c19a-430d-9e65-9140718fcb4c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="11ce1b15-5995-4f89-8454-542f1e930605"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0F0E3E-AAE2-4269-B402-B7C42270AD4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{755A2082-2DEF-4DFD-A722-00F032A28139}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4572,4 +5569,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0F0E3E-AAE2-4269-B402-B7C42270AD4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{258C3525-B843-4DF1-AAB7-9A7C9FE670BA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a49ec6c6-c19a-430d-9e65-9140718fcb4c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="11ce1b15-5995-4f89-8454-542f1e930605"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Latest update of the list
</commit_message>
<xml_diff>
--- a/Data/DS courses list.xlsx
+++ b/Data/DS courses list.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ola\OneDrive - Universiteit Utrecht\Documents\GitHub\UU-DS-courses\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F5F4F4-273D-4BC6-914B-FAB1F571B413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766F6BC5-5435-465C-A505-CCB750D8C9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1020" yWindow="-13140" windowWidth="28965" windowHeight="11730" xr2:uid="{1526A550-0408-4384-9B3B-2B5C51FB6CCB}"/>
+    <workbookView xWindow="1500" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{1526A550-0408-4384-9B3B-2B5C51FB6CCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AZ$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AZ$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,6 @@
     <author>tc={55636430-28F9-427E-8FC9-0523E795980C}</author>
     <author>tc={4D3D460E-D00C-48E4-97F6-28235A8C037F}</author>
     <author>tc={2C1CB73F-0B60-41E5-AECE-1427034B9CE3}</author>
-    <author>tc={35885A4E-3B89-4D6A-95CD-08862DFB9430}</author>
     <author>tc={0477E9A7-5E83-41B8-965E-BC68BE4572C4}</author>
     <author>tc={E2FFAAF8-7744-465F-9701-9A2AFF0D8FD2}</author>
     <author>tc={971B0614-288D-4052-BBD0-23AC10C52401}</author>
@@ -56,6 +55,14 @@
     <author>tc={D9A68AAD-F7F5-48E9-86BF-E791855CE074}</author>
     <author>tc={D2CE96B7-DA8C-4491-9962-80A041D6783C}</author>
     <author>tc={0156854D-B856-40C8-9F6A-56D1A73DF7D0}</author>
+    <author>tc={8DC05F39-DC0F-403F-BD0D-9805E4149521}</author>
+    <author>tc={20009BA8-38A7-46E2-A547-E42B8BC3C6F9}</author>
+    <author>tc={76797D44-E9B7-4CA4-8DB3-ECF16F3623E0}</author>
+    <author>tc={B09121BD-C6B9-45B7-B068-F72C4CE45557}</author>
+    <author>tc={224FC773-6FA8-4FE7-BE1E-211C4660CC01}</author>
+    <author>tc={DC32272E-33B4-4E2C-8CF3-39D3CC2DB77C}</author>
+    <author>tc={FE67C216-38D7-4D76-8ABE-630EFFE97066}</author>
+    <author>tc={7B8D548D-F7CB-48BF-9340-F1F91B2165A2}</author>
   </authors>
   <commentList>
     <comment ref="AO1" authorId="0" shapeId="0" xr:uid="{7912B0EA-387D-478B-95D3-9090A6112730}">
@@ -117,15 +124,7 @@
     using these data for estimation purposes</t>
       </text>
     </comment>
-    <comment ref="A35" authorId="5" shapeId="0" xr:uid="{35885A4E-3B89-4D6A-95CD-08862DFB9430}">
-      <text>
-        <t>[Komentarz podzielony na wątki]
-Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
-Komentarz:
-    The course covers the essentials of qualitative research, in particular techniques for identifying themes, the making of systematic comparisons, and grounding interpretation in theory. Finally, it focuses on the principles of dovetailing primary ethnographic research, secondary data, and larger theoretical frames.</t>
-      </text>
-    </comment>
-    <comment ref="AO49" authorId="6" shapeId="0" xr:uid="{0477E9A7-5E83-41B8-965E-BC68BE4572C4}">
+    <comment ref="AO47" authorId="5" shapeId="0" xr:uid="{0477E9A7-5E83-41B8-965E-BC68BE4572C4}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -133,7 +132,7 @@
     inference</t>
       </text>
     </comment>
-    <comment ref="A55" authorId="7" shapeId="0" xr:uid="{E2FFAAF8-7744-465F-9701-9A2AFF0D8FD2}">
+    <comment ref="A53" authorId="6" shapeId="0" xr:uid="{E2FFAAF8-7744-465F-9701-9A2AFF0D8FD2}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -141,7 +140,7 @@
     This course mentions in discription a statistical software use but I'm not sure what it is</t>
       </text>
     </comment>
-    <comment ref="AR62" authorId="8" shapeId="0" xr:uid="{971B0614-288D-4052-BBD0-23AC10C52401}">
+    <comment ref="AR60" authorId="7" shapeId="0" xr:uid="{971B0614-288D-4052-BBD0-23AC10C52401}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -149,7 +148,7 @@
     qualitative data</t>
       </text>
     </comment>
-    <comment ref="AU62" authorId="9" shapeId="0" xr:uid="{7C5818E2-1E6A-4677-95FD-D0E0F1BC44BF}">
+    <comment ref="AU60" authorId="8" shapeId="0" xr:uid="{7C5818E2-1E6A-4677-95FD-D0E0F1BC44BF}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -157,7 +156,7 @@
     The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</t>
       </text>
     </comment>
-    <comment ref="A63" authorId="10" shapeId="0" xr:uid="{0F9D3427-B4EC-4231-A8B8-1CD7AE2C5236}">
+    <comment ref="A61" authorId="9" shapeId="0" xr:uid="{0F9D3427-B4EC-4231-A8B8-1CD7AE2C5236}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -167,7 +166,7 @@
     only spss mantioned in the literature</t>
       </text>
     </comment>
-    <comment ref="AR64" authorId="11" shapeId="0" xr:uid="{B346AB8C-D5F8-4A60-B1CA-15714598AC1D}">
+    <comment ref="AR62" authorId="10" shapeId="0" xr:uid="{B346AB8C-D5F8-4A60-B1CA-15714598AC1D}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -175,7 +174,7 @@
     qualitative data</t>
       </text>
     </comment>
-    <comment ref="AU64" authorId="12" shapeId="0" xr:uid="{FA9CD2C0-F5EE-473A-BF68-EE1E51FD7EED}">
+    <comment ref="AU62" authorId="11" shapeId="0" xr:uid="{FA9CD2C0-F5EE-473A-BF68-EE1E51FD7EED}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -183,7 +182,7 @@
     The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</t>
       </text>
     </comment>
-    <comment ref="AR65" authorId="13" shapeId="0" xr:uid="{74E5C956-2E55-47CF-908B-6DF2CA8BFF70}">
+    <comment ref="AR63" authorId="12" shapeId="0" xr:uid="{74E5C956-2E55-47CF-908B-6DF2CA8BFF70}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -191,7 +190,7 @@
     qualitative data</t>
       </text>
     </comment>
-    <comment ref="AU65" authorId="14" shapeId="0" xr:uid="{D9A68AAD-F7F5-48E9-86BF-E791855CE074}">
+    <comment ref="AU63" authorId="13" shapeId="0" xr:uid="{D9A68AAD-F7F5-48E9-86BF-E791855CE074}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -199,7 +198,7 @@
     The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</t>
       </text>
     </comment>
-    <comment ref="AR66" authorId="15" shapeId="0" xr:uid="{D2CE96B7-DA8C-4491-9962-80A041D6783C}">
+    <comment ref="AR64" authorId="14" shapeId="0" xr:uid="{D2CE96B7-DA8C-4491-9962-80A041D6783C}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -207,7 +206,7 @@
     The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</t>
       </text>
     </comment>
-    <comment ref="AU66" authorId="16" shapeId="0" xr:uid="{0156854D-B856-40C8-9F6A-56D1A73DF7D0}">
+    <comment ref="AU64" authorId="15" shapeId="0" xr:uid="{0156854D-B856-40C8-9F6A-56D1A73DF7D0}">
       <text>
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
@@ -215,12 +214,89 @@
     The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</t>
       </text>
     </comment>
+    <comment ref="H67" authorId="16" shapeId="0" xr:uid="{8DC05F39-DC0F-403F-BD0D-9805E4149521}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    he is not anymore but still in osiris</t>
+      </text>
+    </comment>
+    <comment ref="S70" authorId="17" shapeId="0" xr:uid="{20009BA8-38A7-46E2-A547-E42B8BC3C6F9}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    ethics of a research</t>
+      </text>
+    </comment>
+    <comment ref="A74" authorId="18" shapeId="0" xr:uid="{76797D44-E9B7-4CA4-8DB3-ECF16F3623E0}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    This course is hard to asses for me 
+After taking this course, the student will be able to:
+Independently build an experiment on the computer.
+Analyse data from self-built experiment using a computer.
+These skills are indispensable for undergraduate research.
+Relationship between tests and learning objectives
+The test consists of making assignments in which experiments are developed and data are analysed.
+Content
+In this course, students acquire skills needed to set up a psychological experiment. The practical consists of five assignments. In these assignments, the student develops computer-based experiments and/or questionnaires and carries out data processing. The tools used to set up experiments and perform data processing include a graphical experiment builder and Microsoft Excel.</t>
+      </text>
+    </comment>
+    <comment ref="S76" authorId="19" shapeId="0" xr:uid="{B09121BD-C6B9-45B7-B068-F72C4CE45557}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    To be able to read, describe and interpret quantitative empirical data, tables and graphs on socio-demographic topics
+Apply social science theories to interpret and explain empirical data
+Being able to derive and formulate testable hypotheses</t>
+      </text>
+    </comment>
+    <comment ref="A80" authorId="20" shapeId="0" xr:uid="{224FC773-6FA8-4FE7-BE1E-211C4660CC01}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    Its I think more about qualitative research and its hard to asses. 
+DISCRIPTION
+After students have completed their fieldwork, the main task that needs to go hand-in-hand with writing is the combination of such first-hand research with secondary data (historical, socio-economic, media-based, environmental, legal, etc.), and finally with the larger, more general theoretical questions students set out to answer or the theoretical debate they are addressing. This practical seminar initiates the writing of the M.Sc. thesis, and teaches students how to use their empirical knowledge and secondary materials to develop broader interpretations about their study in a meaningful relationship with the theoretical frame of their research question.
+The course covers the essentials of qualitative research, in particular techniques for identifying themes, the making of systematic comparisons, and grounding interpretation in theory. Finally, it focuses on the principles of dovetailing primary ethnographic research, secondary data, and larger theoretical frames.</t>
+      </text>
+    </comment>
+    <comment ref="A81" authorId="21" shapeId="0" xr:uid="{DC32272E-33B4-4E2C-8CF3-39D3CC2DB77C}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    it is said they analize dataset but it is not mentioned with what tool if any</t>
+      </text>
+    </comment>
+    <comment ref="A85" authorId="22" shapeId="0" xr:uid="{FE67C216-38D7-4D76-8ABE-630EFFE97066}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    This program list "software" I dont know which. In requiraments thay said that basic skils from SPSS, Stata, or R are desired</t>
+      </text>
+    </comment>
+    <comment ref="A90" authorId="23" shapeId="0" xr:uid="{7B8D548D-F7CB-48BF-9340-F1F91B2165A2}">
+      <text>
+        <t>[Komentarz podzielony na wątki]
+Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
+Komentarz:
+    they do theory about neuroscience. There is mentioned an eye tracking dataset interpretation and analysis but there is no explicitly said what is used for that</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="378">
   <si>
     <t>Course Name</t>
   </si>
@@ -809,18 +885,9 @@
     <t>SEM2</t>
   </si>
   <si>
-    <t>Integration of theory and data analysis </t>
-  </si>
-  <si>
-    <t>SEM3</t>
-  </si>
-  <si>
     <t>Cultural Anthropology: Sociocultural Transformation (res) (CSTM)</t>
   </si>
   <si>
-    <t>prof. dr. A.C.G.M. Robben</t>
-  </si>
-  <si>
     <t>Measurement and modelling with social data </t>
   </si>
   <si>
@@ -1164,13 +1231,235 @@
   </si>
   <si>
     <t xml:space="preserve">MSBBSS03 and MSBBSS04 </t>
+  </si>
+  <si>
+    <t>Causal Inference and Structural Equation Modeling</t>
+  </si>
+  <si>
+    <t>prof. dr. E.L. Hamaker</t>
+  </si>
+  <si>
+    <t>prof. dr. E.L. Hamaker, dr. N.K. Schuurman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSBBSS02 and MSBBSS03 and MSBBSS04 </t>
+  </si>
+  <si>
+    <t>Mplus </t>
+  </si>
+  <si>
+    <t>Computational inference with R</t>
+  </si>
+  <si>
+    <t>prof.dr. M.J.C.  Eijkemans</t>
+  </si>
+  <si>
+    <t>dr. P.M. van de Ven</t>
+  </si>
+  <si>
+    <t>Diagnostical Methods in Clinical Psychology</t>
+  </si>
+  <si>
+    <t>drs. J.M. Versteeg</t>
+  </si>
+  <si>
+    <t>Psychopathology (202100181), Psychopathology II (200300181), Psychopathology II (200400293), Psychopathology II (201400181), Psychopathology II (201400182), Psychopathology II (SW980003)</t>
+  </si>
+  <si>
+    <t>Doing Ethnography</t>
+  </si>
+  <si>
+    <t>dr. D. Jovanovic</t>
+  </si>
+  <si>
+    <t>dr. D. Jovanovic, dr. W.M. Sier</t>
+  </si>
+  <si>
+    <t>Cultural Anthropology: Sustainable Citizenship (SCIM)</t>
+  </si>
+  <si>
+    <t>Doing a Qualitative Research Project</t>
+  </si>
+  <si>
+    <t>H.J. Leplaa, MSc</t>
+  </si>
+  <si>
+    <t>Methods and Statistics in the Social Science (SW-MS-MI1), International Perspectives on Youth and Education (SW-PED-MI14), Child and Adolescent Relationships and Development (CARD) (SW-PED-MI13)</t>
+  </si>
+  <si>
+    <t>AR (SOC) (201800024), Applying research methods and statistics (201800028), AR (ISS) (201800025),  Research methods and statistics 2 (200300173), Research Methods and Statistics 2 (201100028), Research methods and statstics 2 (201100025), Research methods and statistics 2 (201100024), Research methods and statistics 2 psych. (200501023), AR (PW &amp; OWW) (201800173), ARM (PSY) (201800055)</t>
+  </si>
+  <si>
+    <t>limited number of participants</t>
+  </si>
+  <si>
+    <t>dr. P.J. Lugtig, Carina Fransen, Barry Schouten, Ton de Waal, Bart Bakker, Peter-Paul de Wolf, Vera Toepoel, Edwin de Jonge</t>
+  </si>
+  <si>
+    <t>Elective Statistical analysis with R</t>
+  </si>
+  <si>
+    <t>EMOS: Core module</t>
+  </si>
+  <si>
+    <t>dr. M.J.L.F. Cruyff</t>
+  </si>
+  <si>
+    <t>Graduate School for Social and Behavioural Sciences of Utrecht University</t>
+  </si>
+  <si>
+    <t>Experimental Methods and Statistics</t>
+  </si>
+  <si>
+    <t>dr. K.E. Overvliet</t>
+  </si>
+  <si>
+    <t>dr. K.E. Overvliet, dr. B. Liefooghe</t>
+  </si>
+  <si>
+    <t>1, 3</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence (CKIB)</t>
+  </si>
+  <si>
+    <t>Experimenting </t>
+  </si>
+  <si>
+    <t>dr. I.T.C. Hooge</t>
+  </si>
+  <si>
+    <t>dr. J.S. Benjamins, dr. R.S. Hessels</t>
+  </si>
+  <si>
+    <t>dr. J.G. de Kruijf</t>
+  </si>
+  <si>
+    <t>Exploring Ethnography</t>
+  </si>
+  <si>
+    <t>Family sociology: trends, theory and quantitative research</t>
+  </si>
+  <si>
+    <t>dr. M.D. Brons</t>
+  </si>
+  <si>
+    <t>dr. M.D. Brons, dr. A. Poortman, dr. Deni Mazrekaj, R.L.F. ten Kate, W.B.P. Kwint</t>
+  </si>
+  <si>
+    <t>Research methods and statistics 2 (201100024), AR (SOC) (201800024)</t>
+  </si>
+  <si>
+    <t>Foundation of research methods and statistics</t>
+  </si>
+  <si>
+    <t>drs. M.A.A. den Otter</t>
+  </si>
+  <si>
+    <t>Social Education and Youth Policy (SW-PED-MI12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fundamentals of statistics </t>
+  </si>
+  <si>
+    <t>dr. D.J. Hessen</t>
+  </si>
+  <si>
+    <t>MSc. L. Boeschoten</t>
+  </si>
+  <si>
+    <t>Integration of theory and data analysis</t>
+  </si>
+  <si>
+    <t>prof. dr. C.G. Koonings</t>
+  </si>
+  <si>
+    <t>Ethnographic fieldwork (201100072)</t>
+  </si>
+  <si>
+    <t>Integrative Practicum I: Research Skills</t>
+  </si>
+  <si>
+    <t>dr. B. Liefooghe</t>
+  </si>
+  <si>
+    <t>dr. C. Zhang</t>
+  </si>
+  <si>
+    <t>Social and Health Psychology (SHPM)</t>
+  </si>
+  <si>
+    <t>Integrative Practicum II: Research Methods</t>
+  </si>
+  <si>
+    <t>dr. H. Marien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrative practical I </t>
+  </si>
+  <si>
+    <t>dr. E. van de Weijer-Bergsma</t>
+  </si>
+  <si>
+    <t>Integrative practical II</t>
+  </si>
+  <si>
+    <t>dr. B. Flunger</t>
+  </si>
+  <si>
+    <t>dr. B. Flunger, prof. dr. Tamara van Gog</t>
+  </si>
+  <si>
+    <t>Internet Social Media and Networks</t>
+  </si>
+  <si>
+    <t>dr. R. Corten, dr. Deni Mazrekaj, dr. L.G.M. Drouhot</t>
+  </si>
+  <si>
+    <t>Sociology: Contemporary Social Problems (ASVM)</t>
+  </si>
+  <si>
+    <t>Applied Cognitive Psychology, Clinical Child and Adolescent Psychology, Clinical Child Family and Education Studies, Clinical Psychology, Sustainable Citizenship, Educational Sciences, Neuropsychology, Social Policy and Public Health, Social Health and Organisational Psychology, Contemporary Social Problems, Youth Education and Society, Youth Studies</t>
+  </si>
+  <si>
+    <t>Introduction to Biomedical Statistics</t>
+  </si>
+  <si>
+    <t>M. Schipper</t>
+  </si>
+  <si>
+    <t>M. Schipper, M. van Smeden, M.J.C. Eijkemans, prof. dr. RM van den Bor</t>
+  </si>
+  <si>
+    <t>Introduction to Cognitive Models</t>
+  </si>
+  <si>
+    <t>Introduction to Multilevel modelling and Psychometrics</t>
+  </si>
+  <si>
+    <t>dr. E. Aarts, dr. D.J. Hessen</t>
+  </si>
+  <si>
+    <t>Multivariate statistics (201300002) and Computational inference with R (201300004) and Fundamentals of statistics (201300008)</t>
+  </si>
+  <si>
+    <t>Introduction to Research Methods and Statistics (PSY) </t>
+  </si>
+  <si>
+    <t>Introduction to educational neuroscience</t>
+  </si>
+  <si>
+    <t>prof. dr. P.P.M. Leseman</t>
+  </si>
+  <si>
+    <t>dr. A. Wijnroks, dr. O. Oudgenoeg-Paz, prof. dr. Tamara van Gog</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1234,12 +1523,6 @@
       <color rgb="FF000000"/>
       <name val="Open Sans"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1635,55 +1918,89 @@
   <threadedComment ref="AO31" dT="2022-10-08T17:47:06.98" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{2C1CB73F-0B60-41E5-AECE-1427034B9CE3}">
     <text>using these data for estimation purposes</text>
   </threadedComment>
-  <threadedComment ref="A35" dT="2022-10-08T18:10:51.15" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{35885A4E-3B89-4D6A-95CD-08862DFB9430}">
-    <text>The course covers the essentials of qualitative research, in particular techniques for identifying themes, the making of systematic comparisons, and grounding interpretation in theory. Finally, it focuses on the principles of dovetailing primary ethnographic research, secondary data, and larger theoretical frames.</text>
-  </threadedComment>
-  <threadedComment ref="AO49" dT="2022-10-11T10:33:57.67" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{0477E9A7-5E83-41B8-965E-BC68BE4572C4}">
+  <threadedComment ref="AO47" dT="2022-10-11T10:33:57.67" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{0477E9A7-5E83-41B8-965E-BC68BE4572C4}">
     <text>inference</text>
   </threadedComment>
-  <threadedComment ref="A55" dT="2022-10-12T09:45:31.51" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{E2FFAAF8-7744-465F-9701-9A2AFF0D8FD2}">
+  <threadedComment ref="A53" dT="2022-10-12T09:45:31.51" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{E2FFAAF8-7744-465F-9701-9A2AFF0D8FD2}">
     <text>This course mentions in discription a statistical software use but I'm not sure what it is</text>
   </threadedComment>
-  <threadedComment ref="AR62" dT="2022-10-12T15:01:51.51" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{971B0614-288D-4052-BBD0-23AC10C52401}">
+  <threadedComment ref="AR60" dT="2022-10-12T15:01:51.51" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{971B0614-288D-4052-BBD0-23AC10C52401}">
     <text>qualitative data</text>
   </threadedComment>
-  <threadedComment ref="AU62" dT="2022-10-12T15:15:59.00" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{7C5818E2-1E6A-4677-95FD-D0E0F1BC44BF}">
+  <threadedComment ref="AU60" dT="2022-10-12T15:15:59.00" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{7C5818E2-1E6A-4677-95FD-D0E0F1BC44BF}">
     <text>The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</text>
   </threadedComment>
-  <threadedComment ref="A63" dT="2022-10-12T15:26:01.31" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{0F9D3427-B4EC-4231-A8B8-1CD7AE2C5236}">
+  <threadedComment ref="A61" dT="2022-10-12T15:26:01.31" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{0F9D3427-B4EC-4231-A8B8-1CD7AE2C5236}">
     <text>no course description</text>
   </threadedComment>
-  <threadedComment ref="A63" dT="2022-10-12T15:26:28.06" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{F121CDAB-DC8B-48D6-9505-C2300F077CB9}" parentId="{0F9D3427-B4EC-4231-A8B8-1CD7AE2C5236}">
+  <threadedComment ref="A61" dT="2022-10-12T15:26:28.06" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{F121CDAB-DC8B-48D6-9505-C2300F077CB9}" parentId="{0F9D3427-B4EC-4231-A8B8-1CD7AE2C5236}">
     <text>only spss mantioned in the literature</text>
   </threadedComment>
-  <threadedComment ref="AR64" dT="2022-10-12T15:29:32.58" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{B346AB8C-D5F8-4A60-B1CA-15714598AC1D}">
+  <threadedComment ref="AR62" dT="2022-10-12T15:29:32.58" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{B346AB8C-D5F8-4A60-B1CA-15714598AC1D}">
     <text>qualitative data</text>
   </threadedComment>
-  <threadedComment ref="AU64" dT="2022-10-12T15:29:11.55" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{FA9CD2C0-F5EE-473A-BF68-EE1E51FD7EED}">
+  <threadedComment ref="AU62" dT="2022-10-12T15:29:11.55" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{FA9CD2C0-F5EE-473A-BF68-EE1E51FD7EED}">
     <text>The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</text>
   </threadedComment>
-  <threadedComment ref="AR65" dT="2022-10-12T15:33:36.58" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{74E5C956-2E55-47CF-908B-6DF2CA8BFF70}">
+  <threadedComment ref="AR63" dT="2022-10-12T15:33:36.58" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{74E5C956-2E55-47CF-908B-6DF2CA8BFF70}">
     <text>qualitative data</text>
   </threadedComment>
-  <threadedComment ref="AU65" dT="2022-10-12T15:33:22.60" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{D9A68AAD-F7F5-48E9-86BF-E791855CE074}">
+  <threadedComment ref="AU63" dT="2022-10-12T15:33:22.60" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{D9A68AAD-F7F5-48E9-86BF-E791855CE074}">
     <text>The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</text>
   </threadedComment>
-  <threadedComment ref="AR66" dT="2022-10-12T15:36:24.67" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{D2CE96B7-DA8C-4491-9962-80A041D6783C}">
+  <threadedComment ref="AR64" dT="2022-10-12T15:36:24.67" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{D2CE96B7-DA8C-4491-9962-80A041D6783C}">
     <text>The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</text>
   </threadedComment>
-  <threadedComment ref="AU66" dT="2022-10-12T15:36:18.72" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{0156854D-B856-40C8-9F6A-56D1A73DF7D0}">
+  <threadedComment ref="AU64" dT="2022-10-12T15:36:18.72" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{0156854D-B856-40C8-9F6A-56D1A73DF7D0}">
     <text>The course is hard to asses becuse the description include "Coding of qualitative data" there is no information how and If thay learn the concepts or that they actually apply that</text>
+  </threadedComment>
+  <threadedComment ref="H67" dT="2022-10-13T16:57:22.75" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{8DC05F39-DC0F-403F-BD0D-9805E4149521}">
+    <text>he is not anymore but still in osiris</text>
+  </threadedComment>
+  <threadedComment ref="S70" dT="2022-10-17T09:51:38.51" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{20009BA8-38A7-46E2-A547-E42B8BC3C6F9}">
+    <text>ethics of a research</text>
+  </threadedComment>
+  <threadedComment ref="A74" dT="2022-10-17T11:08:32.19" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{76797D44-E9B7-4CA4-8DB3-ECF16F3623E0}">
+    <text>This course is hard to asses for me 
+After taking this course, the student will be able to:
+Independently build an experiment on the computer.
+Analyse data from self-built experiment using a computer.
+These skills are indispensable for undergraduate research.
+Relationship between tests and learning objectives
+The test consists of making assignments in which experiments are developed and data are analysed.
+Content
+In this course, students acquire skills needed to set up a psychological experiment. The practical consists of five assignments. In these assignments, the student develops computer-based experiments and/or questionnaires and carries out data processing. The tools used to set up experiments and perform data processing include a graphical experiment builder and Microsoft Excel.</text>
+  </threadedComment>
+  <threadedComment ref="S76" dT="2022-10-17T11:21:30.89" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{B09121BD-C6B9-45B7-B068-F72C4CE45557}">
+    <text>To be able to read, describe and interpret quantitative empirical data, tables and graphs on socio-demographic topics
+Apply social science theories to interpret and explain empirical data
+Being able to derive and formulate testable hypotheses</text>
+  </threadedComment>
+  <threadedComment ref="A80" dT="2022-10-17T11:37:25.89" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{224FC773-6FA8-4FE7-BE1E-211C4660CC01}">
+    <text>Its I think more about qualitative research and its hard to asses. 
+DISCRIPTION
+After students have completed their fieldwork, the main task that needs to go hand-in-hand with writing is the combination of such first-hand research with secondary data (historical, socio-economic, media-based, environmental, legal, etc.), and finally with the larger, more general theoretical questions students set out to answer or the theoretical debate they are addressing. This practical seminar initiates the writing of the M.Sc. thesis, and teaches students how to use their empirical knowledge and secondary materials to develop broader interpretations about their study in a meaningful relationship with the theoretical frame of their research question.
+The course covers the essentials of qualitative research, in particular techniques for identifying themes, the making of systematic comparisons, and grounding interpretation in theory. Finally, it focuses on the principles of dovetailing primary ethnographic research, secondary data, and larger theoretical frames.</text>
+  </threadedComment>
+  <threadedComment ref="A81" dT="2022-10-17T11:40:58.12" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{DC32272E-33B4-4E2C-8CF3-39D3CC2DB77C}">
+    <text>it is said they analize dataset but it is not mentioned with what tool if any</text>
+  </threadedComment>
+  <threadedComment ref="A85" dT="2022-10-17T13:19:44.88" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{FE67C216-38D7-4D76-8ABE-630EFFE97066}">
+    <text>This program list "software" I dont know which. In requiraments thay said that basic skils from SPSS, Stata, or R are desired</text>
+  </threadedComment>
+  <threadedComment ref="A90" dT="2022-10-17T14:27:16.67" personId="{A69B1243-3DE0-4799-B9E4-A811CFD9ED7E}" id="{7B8D548D-F7CB-48BF-9340-F1F91B2165A2}">
+    <text>they do theory about neuroscience. There is mentioned an eye tracking dataset interpretation and analysis but there is no explicitly said what is used for that</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{501E35CE-ACC9-4FC1-9D06-B7BA9C0949C0}">
-  <dimension ref="A1:BE67"/>
+  <dimension ref="A1:BF90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A79" sqref="A79"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1744,7 +2061,7 @@
     <col min="54" max="54" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1800,13 +2117,13 @@
         <v>11</v>
       </c>
       <c r="S1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="T1" t="s">
         <v>64</v>
       </c>
       <c r="U1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="V1" t="s">
         <v>88</v>
@@ -1830,7 +2147,7 @@
         <v>59</v>
       </c>
       <c r="AC1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="AD1" t="s">
         <v>32</v>
@@ -1863,10 +2180,10 @@
         <v>42</v>
       </c>
       <c r="AN1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="AO1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="AP1" t="s">
         <v>50</v>
@@ -1899,25 +2216,28 @@
         <v>173</v>
       </c>
       <c r="AZ1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="BA1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="BB1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="BC1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="BD1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="BE1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1964,7 +2284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2032,7 +2352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -2088,7 +2408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -2141,7 +2461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -2206,7 +2526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -2262,7 +2582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -2312,7 +2632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -2362,7 +2682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -2412,7 +2732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -2462,7 +2782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -2506,7 +2826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>80</v>
       </c>
@@ -2559,7 +2879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -2618,7 +2938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>89</v>
       </c>
@@ -2677,7 +2997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>99</v>
       </c>
@@ -3613,15 +3933,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="34" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B34">
-        <v>202200015</v>
-      </c>
-      <c r="D34" t="s">
-        <v>25</v>
+        <v>201800138</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
       </c>
       <c r="E34" t="s">
         <v>17</v>
@@ -3630,42 +3950,57 @@
         <v>171</v>
       </c>
       <c r="G34" t="s">
-        <v>175</v>
+        <v>192</v>
+      </c>
+      <c r="H34" t="s">
+        <v>193</v>
       </c>
       <c r="I34">
+        <v>7.5</v>
+      </c>
+      <c r="J34">
+        <v>2018</v>
+      </c>
+      <c r="K34">
+        <v>2022</v>
+      </c>
+      <c r="L34">
         <v>2</v>
       </c>
-      <c r="K34">
-        <v>2022</v>
-      </c>
-      <c r="L34" t="s">
-        <v>187</v>
-      </c>
-      <c r="N34">
-        <v>1</v>
-      </c>
-      <c r="P34" t="s">
-        <v>171</v>
+      <c r="M34" t="s">
+        <v>190</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="P34">
+        <v>200300022</v>
       </c>
       <c r="Q34">
         <v>1</v>
       </c>
-      <c r="S34">
-        <v>1</v>
-      </c>
-      <c r="U34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>188</v>
+      <c r="AO34">
+        <v>1</v>
+      </c>
+      <c r="AR34">
+        <v>1</v>
+      </c>
+      <c r="AZ34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>189</v>
       </c>
       <c r="B35">
-        <v>201000091</v>
-      </c>
-      <c r="D35" t="s">
-        <v>25</v>
+        <v>201800139</v>
+      </c>
+      <c r="C35" t="s">
+        <v>194</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
       </c>
       <c r="E35" t="s">
         <v>17</v>
@@ -3673,14 +4008,8 @@
       <c r="F35" t="s">
         <v>171</v>
       </c>
-      <c r="G35" t="s">
-        <v>191</v>
-      </c>
-      <c r="H35" t="s">
-        <v>191</v>
-      </c>
       <c r="I35">
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="J35">
         <v>2018</v>
@@ -3688,22 +4017,16 @@
       <c r="K35">
         <v>2022</v>
       </c>
-      <c r="L35" t="s">
-        <v>189</v>
-      </c>
-      <c r="M35" t="s">
-        <v>190</v>
-      </c>
-      <c r="P35">
-        <v>201100072</v>
-      </c>
-    </row>
-    <row r="36" spans="1:56" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B36">
-        <v>201800138</v>
+        <v>201500130</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -3715,69 +4038,69 @@
         <v>171</v>
       </c>
       <c r="G36" t="s">
-        <v>195</v>
-      </c>
-      <c r="H36" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="I36">
         <v>7.5</v>
       </c>
       <c r="J36">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="K36">
         <v>2022</v>
       </c>
       <c r="L36">
-        <v>2</v>
-      </c>
-      <c r="M36" t="s">
-        <v>193</v>
-      </c>
-      <c r="N36" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="P36">
-        <v>200300022</v>
+        <v>3</v>
+      </c>
+      <c r="N36" t="s">
+        <v>196</v>
+      </c>
+      <c r="P36" t="s">
+        <v>197</v>
       </c>
       <c r="Q36">
         <v>1</v>
       </c>
-      <c r="AO36">
-        <v>1</v>
-      </c>
-      <c r="AR36">
-        <v>1</v>
-      </c>
-      <c r="AZ36">
+      <c r="T36">
+        <v>1</v>
+      </c>
+      <c r="Y36">
+        <v>1</v>
+      </c>
+      <c r="AE36">
+        <v>1</v>
+      </c>
+      <c r="AK36">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="B37">
-        <v>201800139</v>
-      </c>
-      <c r="C37" t="s">
-        <v>197</v>
+        <v>200300022</v>
       </c>
       <c r="D37">
         <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="F37" t="s">
         <v>171</v>
       </c>
+      <c r="G37" t="s">
+        <v>202</v>
+      </c>
+      <c r="H37" t="s">
+        <v>203</v>
+      </c>
       <c r="I37">
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="J37">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="K37">
         <v>2022</v>
@@ -3785,16 +4108,31 @@
       <c r="L37">
         <v>2</v>
       </c>
+      <c r="N37" t="s">
+        <v>200</v>
+      </c>
+      <c r="P37" t="s">
+        <v>201</v>
+      </c>
+      <c r="AO37">
+        <v>1</v>
+      </c>
+      <c r="AR37">
+        <v>1</v>
+      </c>
+      <c r="AZ37">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B38">
-        <v>201500130</v>
-      </c>
-      <c r="D38">
-        <v>3</v>
+        <v>201300001</v>
+      </c>
+      <c r="D38" t="s">
+        <v>25</v>
       </c>
       <c r="E38" t="s">
         <v>17</v>
@@ -3802,9 +4140,6 @@
       <c r="F38" t="s">
         <v>171</v>
       </c>
-      <c r="G38" t="s">
-        <v>201</v>
-      </c>
       <c r="I38">
         <v>7.5</v>
       </c>
@@ -3814,87 +4149,57 @@
       <c r="K38">
         <v>2022</v>
       </c>
-      <c r="L38">
-        <v>3</v>
-      </c>
-      <c r="N38" t="s">
-        <v>199</v>
+      <c r="L38" t="s">
+        <v>154</v>
+      </c>
+      <c r="M38" t="s">
+        <v>205</v>
       </c>
       <c r="P38" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q38">
-        <v>1</v>
-      </c>
-      <c r="T38">
+        <v>171</v>
+      </c>
+      <c r="U38">
         <v>1</v>
       </c>
       <c r="Y38">
         <v>1</v>
       </c>
+      <c r="AA38">
+        <v>1</v>
+      </c>
       <c r="AE38">
         <v>1</v>
       </c>
       <c r="AK38">
         <v>1</v>
       </c>
+      <c r="AO38">
+        <v>1</v>
+      </c>
+      <c r="AQ38">
+        <v>1</v>
+      </c>
+      <c r="AR38">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>202</v>
+      <c r="A39" s="5" t="s">
+        <v>206</v>
       </c>
       <c r="B39">
-        <v>200300022</v>
+        <v>202100022</v>
       </c>
       <c r="D39">
         <v>3</v>
       </c>
-      <c r="E39" t="s">
-        <v>84</v>
-      </c>
-      <c r="F39" t="s">
-        <v>171</v>
-      </c>
-      <c r="G39" t="s">
-        <v>205</v>
-      </c>
-      <c r="H39" t="s">
-        <v>206</v>
-      </c>
-      <c r="I39">
-        <v>7.5</v>
-      </c>
-      <c r="J39">
-        <v>2015</v>
-      </c>
-      <c r="K39">
-        <v>2022</v>
-      </c>
-      <c r="L39">
-        <v>2</v>
-      </c>
-      <c r="N39" t="s">
-        <v>203</v>
-      </c>
-      <c r="P39" t="s">
-        <v>204</v>
-      </c>
-      <c r="AO39">
-        <v>1</v>
-      </c>
-      <c r="AR39">
-        <v>1</v>
-      </c>
-      <c r="AZ39">
-        <v>1</v>
-      </c>
     </row>
     <row r="40" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>208</v>
+      </c>
+      <c r="B40" t="s">
         <v>207</v>
-      </c>
-      <c r="B40">
-        <v>201300001</v>
       </c>
       <c r="D40" t="s">
         <v>25</v>
@@ -3903,68 +4208,146 @@
         <v>17</v>
       </c>
       <c r="F40" t="s">
-        <v>171</v>
+        <v>26</v>
+      </c>
+      <c r="G40" t="s">
+        <v>209</v>
+      </c>
+      <c r="H40" t="s">
+        <v>209</v>
       </c>
       <c r="I40">
         <v>7.5</v>
       </c>
       <c r="J40">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="K40">
         <v>2022</v>
       </c>
-      <c r="L40" t="s">
-        <v>154</v>
+      <c r="L40">
+        <v>1</v>
       </c>
       <c r="M40" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="P40" t="s">
-        <v>171</v>
-      </c>
-      <c r="U40">
-        <v>1</v>
-      </c>
-      <c r="Y40">
+        <v>25</v>
+      </c>
+      <c r="Q40">
+        <v>1</v>
+      </c>
+      <c r="Z40">
         <v>1</v>
       </c>
       <c r="AA40">
         <v>1</v>
       </c>
-      <c r="AE40">
-        <v>1</v>
-      </c>
       <c r="AK40">
         <v>1</v>
       </c>
+      <c r="AL40">
+        <v>1</v>
+      </c>
       <c r="AO40">
         <v>1</v>
       </c>
       <c r="AQ40">
         <v>1</v>
       </c>
-      <c r="AR40">
+      <c r="AU40">
+        <v>1</v>
+      </c>
+      <c r="AW40">
+        <v>1</v>
+      </c>
+      <c r="AY40">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="B41">
-        <v>202100022</v>
-      </c>
-      <c r="D41">
-        <v>3</v>
+      <c r="A41" t="s">
+        <v>211</v>
+      </c>
+      <c r="B41" t="s">
+        <v>212</v>
+      </c>
+      <c r="D41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41" t="s">
+        <v>26</v>
+      </c>
+      <c r="G41" t="s">
+        <v>183</v>
+      </c>
+      <c r="H41" t="s">
+        <v>183</v>
+      </c>
+      <c r="I41">
+        <v>7.5</v>
+      </c>
+      <c r="J41">
+        <v>2021</v>
+      </c>
+      <c r="K41">
+        <v>2022</v>
+      </c>
+      <c r="L41">
+        <v>2</v>
+      </c>
+      <c r="M41" t="s">
+        <v>213</v>
+      </c>
+      <c r="P41" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q41">
+        <v>1</v>
+      </c>
+      <c r="Z41">
+        <v>1</v>
+      </c>
+      <c r="AA41">
+        <v>1</v>
+      </c>
+      <c r="AB41">
+        <v>1</v>
+      </c>
+      <c r="AC41">
+        <v>1</v>
+      </c>
+      <c r="AD41">
+        <v>1</v>
+      </c>
+      <c r="AE41">
+        <v>1</v>
+      </c>
+      <c r="AK41">
+        <v>1</v>
+      </c>
+      <c r="AO41">
+        <v>1</v>
+      </c>
+      <c r="AU41">
+        <v>1</v>
+      </c>
+      <c r="AW41">
+        <v>1</v>
+      </c>
+      <c r="AY41">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>211</v>
-      </c>
-      <c r="B42" t="s">
-        <v>210</v>
+        <v>218</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>214</v>
       </c>
       <c r="D42" t="s">
         <v>25</v>
@@ -3973,134 +4356,68 @@
         <v>17</v>
       </c>
       <c r="F42" t="s">
-        <v>26</v>
+        <v>171</v>
       </c>
       <c r="G42" t="s">
-        <v>212</v>
-      </c>
-      <c r="H42" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="I42">
-        <v>7.5</v>
-      </c>
-      <c r="J42">
-        <v>2021</v>
+        <v>1.5</v>
       </c>
       <c r="K42">
         <v>2022</v>
       </c>
-      <c r="L42">
-        <v>1</v>
-      </c>
-      <c r="M42" t="s">
-        <v>213</v>
-      </c>
-      <c r="P42" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q42">
-        <v>1</v>
-      </c>
-      <c r="Z42">
-        <v>1</v>
-      </c>
-      <c r="AA42">
+      <c r="R42" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="AC42">
+        <v>1</v>
+      </c>
+      <c r="AE42">
+        <v>1</v>
+      </c>
+      <c r="AG42">
         <v>1</v>
       </c>
       <c r="AK42">
-        <v>1</v>
-      </c>
-      <c r="AL42">
-        <v>1</v>
-      </c>
-      <c r="AO42">
-        <v>1</v>
-      </c>
-      <c r="AQ42">
-        <v>1</v>
-      </c>
-      <c r="AU42">
-        <v>1</v>
-      </c>
-      <c r="AW42">
-        <v>1</v>
-      </c>
-      <c r="AY42">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B43" t="s">
-        <v>215</v>
-      </c>
-      <c r="D43" t="s">
-        <v>25</v>
+        <v>219</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
       </c>
       <c r="E43" t="s">
         <v>17</v>
       </c>
       <c r="F43" t="s">
-        <v>26</v>
+        <v>171</v>
       </c>
       <c r="G43" t="s">
-        <v>183</v>
+        <v>221</v>
       </c>
       <c r="H43" t="s">
-        <v>183</v>
+        <v>222</v>
       </c>
       <c r="I43">
-        <v>7.5</v>
-      </c>
-      <c r="J43">
-        <v>2021</v>
+        <v>1.5</v>
       </c>
       <c r="K43">
         <v>2022</v>
       </c>
-      <c r="L43">
-        <v>2</v>
-      </c>
-      <c r="M43" t="s">
-        <v>216</v>
-      </c>
-      <c r="P43" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q43">
-        <v>1</v>
-      </c>
-      <c r="Z43">
-        <v>1</v>
-      </c>
-      <c r="AA43">
-        <v>1</v>
-      </c>
-      <c r="AB43">
-        <v>1</v>
-      </c>
-      <c r="AC43">
-        <v>1</v>
-      </c>
-      <c r="AD43">
-        <v>1</v>
+      <c r="R43" s="7" t="s">
+        <v>215</v>
       </c>
       <c r="AE43">
         <v>1</v>
       </c>
-      <c r="AK43">
-        <v>1</v>
-      </c>
-      <c r="AO43">
-        <v>1</v>
-      </c>
-      <c r="AU43">
-        <v>1</v>
-      </c>
-      <c r="AW43">
+      <c r="AG43">
         <v>1</v>
       </c>
       <c r="AY43">
@@ -4109,22 +4426,25 @@
     </row>
     <row r="44" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>221</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="D44" t="s">
-        <v>25</v>
+        <v>224</v>
+      </c>
+      <c r="B44" t="s">
+        <v>225</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
       </c>
       <c r="E44" t="s">
         <v>17</v>
       </c>
       <c r="F44" t="s">
-        <v>171</v>
+        <v>26</v>
       </c>
       <c r="G44" t="s">
-        <v>226</v>
+        <v>231</v>
+      </c>
+      <c r="H44" t="s">
+        <v>231</v>
       </c>
       <c r="I44">
         <v>1.5</v>
@@ -4132,31 +4452,28 @@
       <c r="K44">
         <v>2022</v>
       </c>
-      <c r="R44" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="AC44">
-        <v>1</v>
+      <c r="R44" t="s">
+        <v>228</v>
       </c>
       <c r="AE44">
         <v>1</v>
       </c>
-      <c r="AG44">
-        <v>1</v>
-      </c>
-      <c r="AK44">
+      <c r="AY44">
+        <v>1</v>
+      </c>
+      <c r="BA44">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B45" t="s">
-        <v>222</v>
-      </c>
-      <c r="D45">
-        <v>3</v>
+        <v>227</v>
+      </c>
+      <c r="D45" t="s">
+        <v>25</v>
       </c>
       <c r="E45" t="s">
         <v>17</v>
@@ -4165,10 +4482,10 @@
         <v>171</v>
       </c>
       <c r="G45" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="H45" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="I45">
         <v>1.5</v>
@@ -4176,13 +4493,34 @@
       <c r="K45">
         <v>2022</v>
       </c>
-      <c r="R45" s="7" t="s">
-        <v>218</v>
+      <c r="O45">
+        <v>60</v>
+      </c>
+      <c r="R45" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z45">
+        <v>1</v>
+      </c>
+      <c r="AA45">
+        <v>1</v>
       </c>
       <c r="AE45">
         <v>1</v>
       </c>
-      <c r="AG45">
+      <c r="AK45">
+        <v>1</v>
+      </c>
+      <c r="AO45">
+        <v>1</v>
+      </c>
+      <c r="AQ45">
+        <v>1</v>
+      </c>
+      <c r="AU45">
+        <v>1</v>
+      </c>
+      <c r="AW45">
         <v>1</v>
       </c>
       <c r="AY45">
@@ -4191,25 +4529,25 @@
     </row>
     <row r="46" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B46" t="s">
-        <v>228</v>
-      </c>
-      <c r="D46">
-        <v>3</v>
+        <v>230</v>
+      </c>
+      <c r="D46" t="s">
+        <v>25</v>
       </c>
       <c r="E46" t="s">
         <v>17</v>
       </c>
       <c r="F46" t="s">
-        <v>26</v>
+        <v>171</v>
       </c>
       <c r="G46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I46">
         <v>1.5</v>
@@ -4217,25 +4555,49 @@
       <c r="K46">
         <v>2022</v>
       </c>
+      <c r="O46">
+        <v>80</v>
+      </c>
       <c r="R46" t="s">
-        <v>231</v>
+        <v>220</v>
+      </c>
+      <c r="Z46">
+        <v>1</v>
+      </c>
+      <c r="AA46">
+        <v>1</v>
+      </c>
+      <c r="AB46">
+        <v>1</v>
       </c>
       <c r="AE46">
         <v>1</v>
       </c>
+      <c r="AG46">
+        <v>1</v>
+      </c>
+      <c r="AO46">
+        <v>1</v>
+      </c>
+      <c r="AR46">
+        <v>1</v>
+      </c>
+      <c r="AU46">
+        <v>1</v>
+      </c>
       <c r="AY46">
         <v>1</v>
       </c>
-      <c r="BA46">
+      <c r="BD46">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B47" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D47" t="s">
         <v>25</v>
@@ -4247,10 +4609,10 @@
         <v>171</v>
       </c>
       <c r="G47" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H47" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="I47">
         <v>1.5</v>
@@ -4259,15 +4621,12 @@
         <v>2022</v>
       </c>
       <c r="O47">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="R47" t="s">
-        <v>218</v>
-      </c>
-      <c r="Z47">
-        <v>1</v>
-      </c>
-      <c r="AA47">
+        <v>238</v>
+      </c>
+      <c r="Y47">
         <v>1</v>
       </c>
       <c r="AE47">
@@ -4279,10 +4638,7 @@
       <c r="AO47">
         <v>1</v>
       </c>
-      <c r="AQ47">
-        <v>1</v>
-      </c>
-      <c r="AU47">
+      <c r="AR47">
         <v>1</v>
       </c>
       <c r="AW47">
@@ -4294,10 +4650,10 @@
     </row>
     <row r="48" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="B48" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D48" t="s">
         <v>25</v>
@@ -4309,10 +4665,10 @@
         <v>171</v>
       </c>
       <c r="G48" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="H48" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="I48">
         <v>1.5</v>
@@ -4324,48 +4680,36 @@
         <v>80</v>
       </c>
       <c r="R48" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z48">
-        <v>1</v>
-      </c>
-      <c r="AA48">
-        <v>1</v>
-      </c>
-      <c r="AB48">
-        <v>1</v>
+        <v>242</v>
       </c>
       <c r="AE48">
         <v>1</v>
       </c>
-      <c r="AG48">
+      <c r="AK48">
         <v>1</v>
       </c>
       <c r="AO48">
         <v>1</v>
       </c>
-      <c r="AR48">
-        <v>1</v>
-      </c>
-      <c r="AU48">
+      <c r="AS48">
+        <v>1</v>
+      </c>
+      <c r="AW48">
         <v>1</v>
       </c>
       <c r="AY48">
         <v>1</v>
       </c>
-      <c r="BD48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:57" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>238</v>
-      </c>
-      <c r="B49" t="s">
-        <v>237</v>
-      </c>
-      <c r="D49" t="s">
-        <v>25</v>
+        <v>243</v>
+      </c>
+      <c r="B49">
+        <v>202100012</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
       </c>
       <c r="E49" t="s">
         <v>17</v>
@@ -4374,51 +4718,42 @@
         <v>171</v>
       </c>
       <c r="G49" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="H49" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="I49">
-        <v>1.5</v>
+        <v>7.5</v>
+      </c>
+      <c r="J49">
+        <v>2021</v>
       </c>
       <c r="K49">
         <v>2022</v>
       </c>
-      <c r="O49">
-        <v>50</v>
-      </c>
-      <c r="R49" t="s">
-        <v>241</v>
-      </c>
-      <c r="Y49">
-        <v>1</v>
-      </c>
-      <c r="AE49">
-        <v>1</v>
-      </c>
-      <c r="AK49">
-        <v>1</v>
-      </c>
-      <c r="AO49">
-        <v>1</v>
-      </c>
-      <c r="AR49">
-        <v>1</v>
-      </c>
-      <c r="AW49">
-        <v>1</v>
-      </c>
-      <c r="AY49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="L49">
+        <v>4</v>
+      </c>
+      <c r="N49" t="s">
+        <v>246</v>
+      </c>
+      <c r="P49" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q49">
+        <v>1</v>
+      </c>
+      <c r="S49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B50" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="D50" t="s">
         <v>25</v>
@@ -4427,174 +4762,177 @@
         <v>17</v>
       </c>
       <c r="F50" t="s">
-        <v>171</v>
+        <v>26</v>
       </c>
       <c r="G50" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="H50" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="I50">
-        <v>1.5</v>
+        <v>7.5</v>
+      </c>
+      <c r="J50">
+        <v>2015</v>
       </c>
       <c r="K50">
         <v>2022</v>
       </c>
-      <c r="O50">
-        <v>80</v>
-      </c>
-      <c r="R50" t="s">
-        <v>245</v>
-      </c>
-      <c r="AE50">
-        <v>1</v>
-      </c>
-      <c r="AK50">
-        <v>1</v>
-      </c>
-      <c r="AO50">
-        <v>1</v>
-      </c>
-      <c r="AS50">
-        <v>1</v>
-      </c>
-      <c r="AW50">
-        <v>1</v>
-      </c>
-      <c r="AY50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="L50">
+        <v>4</v>
+      </c>
+      <c r="N50" t="s">
+        <v>108</v>
+      </c>
+      <c r="P50" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q50">
+        <v>1</v>
+      </c>
+      <c r="BB50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>246</v>
-      </c>
-      <c r="B51">
-        <v>202100012</v>
-      </c>
-      <c r="D51">
-        <v>2</v>
-      </c>
-      <c r="E51" t="s">
-        <v>17</v>
-      </c>
-      <c r="F51" t="s">
-        <v>171</v>
-      </c>
-      <c r="G51" t="s">
-        <v>247</v>
-      </c>
-      <c r="H51" t="s">
-        <v>248</v>
-      </c>
-      <c r="I51">
-        <v>7.5</v>
-      </c>
-      <c r="J51">
-        <v>2021</v>
-      </c>
-      <c r="K51">
-        <v>2022</v>
-      </c>
-      <c r="L51">
-        <v>4</v>
-      </c>
-      <c r="N51" t="s">
-        <v>249</v>
-      </c>
-      <c r="P51" t="s">
-        <v>250</v>
-      </c>
-      <c r="Q51">
-        <v>1</v>
-      </c>
-      <c r="S51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:57" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+      <c r="B51" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="52" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>251</v>
-      </c>
-      <c r="B52" t="s">
-        <v>252</v>
-      </c>
-      <c r="D52" t="s">
-        <v>25</v>
+        <v>254</v>
+      </c>
+      <c r="B52">
+        <v>201900025</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="F52" t="s">
-        <v>26</v>
+        <v>171</v>
       </c>
       <c r="G52" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="H52" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="I52">
         <v>7.5</v>
       </c>
-      <c r="J52">
-        <v>2015</v>
+      <c r="J52" t="s">
+        <v>256</v>
       </c>
       <c r="K52">
         <v>2022</v>
       </c>
       <c r="L52">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N52" t="s">
-        <v>108</v>
-      </c>
-      <c r="P52" t="s">
-        <v>25</v>
+        <v>170</v>
+      </c>
+      <c r="P52" s="8" t="s">
+        <v>257</v>
       </c>
       <c r="Q52">
         <v>1</v>
       </c>
-      <c r="BB52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="S52">
+        <v>1</v>
+      </c>
+      <c r="AO52">
+        <v>1</v>
+      </c>
+      <c r="AV52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>255</v>
-      </c>
-      <c r="B53" t="s">
+        <v>260</v>
+      </c>
+      <c r="B53">
+        <v>202200104</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53" t="s">
+        <v>17</v>
+      </c>
+      <c r="F53" t="s">
+        <v>171</v>
+      </c>
+      <c r="G53" t="s">
+        <v>261</v>
+      </c>
+      <c r="H53" t="s">
+        <v>262</v>
+      </c>
+      <c r="I53">
+        <v>7.5</v>
+      </c>
+      <c r="J53" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="54" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="K53">
+        <v>2022</v>
+      </c>
+      <c r="L53">
+        <v>2</v>
+      </c>
+      <c r="P53" t="s">
+        <v>263</v>
+      </c>
+      <c r="S53">
+        <v>1</v>
+      </c>
+      <c r="AN53">
+        <v>1</v>
+      </c>
+      <c r="AO53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="B54">
-        <v>201900025</v>
+        <v>201800032</v>
+      </c>
+      <c r="C54" t="s">
+        <v>265</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="F54" t="s">
         <v>171</v>
       </c>
       <c r="G54" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="H54" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="I54">
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="J54" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="K54">
         <v>2022</v>
@@ -4602,34 +4940,22 @@
       <c r="L54">
         <v>1</v>
       </c>
-      <c r="N54" t="s">
-        <v>170</v>
-      </c>
-      <c r="P54" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q54">
-        <v>1</v>
-      </c>
       <c r="S54">
         <v>1</v>
       </c>
       <c r="AO54">
         <v>1</v>
       </c>
-      <c r="AV54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:57" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B55">
-        <v>202200104</v>
+        <v>200300009</v>
       </c>
       <c r="D55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E55" t="s">
         <v>17</v>
@@ -4638,48 +4964,45 @@
         <v>171</v>
       </c>
       <c r="G55" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="H55" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="I55">
         <v>7.5</v>
       </c>
       <c r="J55" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="K55">
         <v>2022</v>
       </c>
       <c r="L55">
-        <v>2</v>
-      </c>
-      <c r="P55" t="s">
-        <v>266</v>
+        <v>1</v>
+      </c>
+      <c r="N55" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q55">
+        <v>1</v>
       </c>
       <c r="S55">
         <v>1</v>
       </c>
-      <c r="AN55">
-        <v>1</v>
-      </c>
       <c r="AO55">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B56">
-        <v>201800032</v>
-      </c>
-      <c r="C56" t="s">
-        <v>268</v>
-      </c>
-      <c r="D56">
-        <v>2</v>
+        <v>200600027</v>
+      </c>
+      <c r="D56" t="s">
+        <v>25</v>
       </c>
       <c r="E56" t="s">
         <v>17</v>
@@ -4688,21 +5011,30 @@
         <v>171</v>
       </c>
       <c r="G56" t="s">
-        <v>269</v>
-      </c>
-      <c r="H56" t="s">
-        <v>271</v>
+        <v>272</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>286</v>
       </c>
       <c r="I56">
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="J56" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="K56">
         <v>2022</v>
       </c>
-      <c r="L56">
+      <c r="L56" t="s">
+        <v>187</v>
+      </c>
+      <c r="M56" t="s">
+        <v>273</v>
+      </c>
+      <c r="P56" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q56">
         <v>1</v>
       </c>
       <c r="S56">
@@ -4711,43 +5043,58 @@
       <c r="AO56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="AY56">
+        <v>1</v>
+      </c>
+      <c r="AZ56">
+        <v>1</v>
+      </c>
+      <c r="BC56">
+        <v>1</v>
+      </c>
+      <c r="BF56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="B57">
-        <v>200300009</v>
+        <v>201900054</v>
       </c>
       <c r="D57">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E57" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="F57" t="s">
         <v>171</v>
       </c>
       <c r="G57" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="H57" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="I57">
         <v>7.5</v>
       </c>
       <c r="J57" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="K57">
         <v>2022</v>
       </c>
       <c r="L57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N57" t="s">
-        <v>273</v>
+        <v>280</v>
+      </c>
+      <c r="P57" t="s">
+        <v>283</v>
       </c>
       <c r="Q57">
         <v>1</v>
@@ -4759,45 +5106,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="B58">
-        <v>200600027</v>
-      </c>
-      <c r="D58" t="s">
-        <v>25</v>
+        <v>201900398</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
       </c>
       <c r="E58" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="F58" t="s">
         <v>171</v>
       </c>
       <c r="G58" t="s">
-        <v>275</v>
-      </c>
-      <c r="H58" s="8" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="I58">
         <v>7.5</v>
       </c>
       <c r="J58" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="K58">
         <v>2022</v>
       </c>
-      <c r="L58" t="s">
-        <v>187</v>
-      </c>
-      <c r="M58" t="s">
-        <v>276</v>
+      <c r="L58">
+        <v>2</v>
       </c>
       <c r="P58" t="s">
-        <v>171</v>
+        <v>283</v>
       </c>
       <c r="Q58">
         <v>1</v>
@@ -4808,75 +5149,72 @@
       <c r="AO58">
         <v>1</v>
       </c>
-      <c r="AY58">
-        <v>1</v>
-      </c>
-      <c r="AZ58">
-        <v>1</v>
-      </c>
-      <c r="BC58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:57" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="B59">
-        <v>201900054</v>
-      </c>
-      <c r="D59">
-        <v>3</v>
+        <v>200600023</v>
+      </c>
+      <c r="D59" t="s">
+        <v>25</v>
       </c>
       <c r="E59" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="F59" t="s">
         <v>171</v>
       </c>
       <c r="G59" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="H59" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="I59">
         <v>7.5</v>
       </c>
       <c r="J59" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="K59">
         <v>2022</v>
       </c>
-      <c r="L59">
+      <c r="L59" t="s">
+        <v>154</v>
+      </c>
+      <c r="M59" t="s">
+        <v>273</v>
+      </c>
+      <c r="P59" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q59">
+        <v>1</v>
+      </c>
+      <c r="S59">
+        <v>1</v>
+      </c>
+      <c r="AO59">
+        <v>1</v>
+      </c>
+      <c r="AY59">
+        <v>1</v>
+      </c>
+      <c r="AZ59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>292</v>
+      </c>
+      <c r="B60">
+        <v>201800055</v>
+      </c>
+      <c r="D60">
         <v>2</v>
-      </c>
-      <c r="N59" t="s">
-        <v>283</v>
-      </c>
-      <c r="P59" t="s">
-        <v>286</v>
-      </c>
-      <c r="Q59">
-        <v>1</v>
-      </c>
-      <c r="S59">
-        <v>1</v>
-      </c>
-      <c r="AO59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>284</v>
-      </c>
-      <c r="B60">
-        <v>201900398</v>
-      </c>
-      <c r="D60">
-        <v>3</v>
       </c>
       <c r="E60" t="s">
         <v>84</v>
@@ -4885,95 +5223,89 @@
         <v>171</v>
       </c>
       <c r="G60" t="s">
-        <v>285</v>
+        <v>277</v>
+      </c>
+      <c r="H60" t="s">
+        <v>291</v>
       </c>
       <c r="I60">
         <v>7.5</v>
       </c>
       <c r="J60" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="K60">
         <v>2022</v>
       </c>
       <c r="L60">
+        <v>3</v>
+      </c>
+      <c r="P60" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q60">
+        <v>1</v>
+      </c>
+      <c r="S60">
+        <v>1</v>
+      </c>
+      <c r="U60">
+        <v>1</v>
+      </c>
+      <c r="AR60">
+        <v>1</v>
+      </c>
+      <c r="AU60">
+        <v>1</v>
+      </c>
+      <c r="BE60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>293</v>
+      </c>
+      <c r="B61">
+        <v>201800028</v>
+      </c>
+      <c r="D61">
         <v>2</v>
       </c>
-      <c r="P60" t="s">
-        <v>286</v>
-      </c>
-      <c r="Q60">
-        <v>1</v>
-      </c>
-      <c r="S60">
-        <v>1</v>
-      </c>
-      <c r="AO60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>287</v>
-      </c>
-      <c r="B61">
-        <v>200600023</v>
-      </c>
-      <c r="D61" t="s">
-        <v>25</v>
-      </c>
       <c r="E61" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="F61" t="s">
         <v>171</v>
       </c>
       <c r="G61" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="H61" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="I61">
         <v>7.5</v>
       </c>
       <c r="J61" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="K61">
         <v>2022</v>
       </c>
-      <c r="L61" t="s">
-        <v>154</v>
-      </c>
-      <c r="M61" t="s">
-        <v>276</v>
+      <c r="L61">
+        <v>3</v>
       </c>
       <c r="P61" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q61">
-        <v>1</v>
-      </c>
-      <c r="S61">
-        <v>1</v>
-      </c>
-      <c r="AO61">
-        <v>1</v>
-      </c>
-      <c r="AY61">
-        <v>1</v>
-      </c>
-      <c r="AZ61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:57" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="62" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B62">
-        <v>201800055</v>
+        <v>201800173</v>
       </c>
       <c r="D62">
         <v>2</v>
@@ -4985,28 +5317,22 @@
         <v>171</v>
       </c>
       <c r="G62" t="s">
-        <v>280</v>
-      </c>
-      <c r="H62" t="s">
         <v>294</v>
       </c>
       <c r="I62">
         <v>7.5</v>
       </c>
       <c r="J62" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="K62">
         <v>2022</v>
       </c>
       <c r="L62">
-        <v>3</v>
-      </c>
-      <c r="P62" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q62">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="P62">
+        <v>201800171</v>
       </c>
       <c r="S62">
         <v>1</v>
@@ -5024,12 +5350,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B63">
-        <v>201800028</v>
+        <v>201800025</v>
       </c>
       <c r="D63">
         <v>2</v>
@@ -5041,16 +5367,16 @@
         <v>171</v>
       </c>
       <c r="G63" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H63" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I63">
         <v>7.5</v>
       </c>
       <c r="J63" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="K63">
         <v>2022</v>
@@ -5058,16 +5384,37 @@
       <c r="L63">
         <v>3</v>
       </c>
-      <c r="P63" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="64" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="N63" t="s">
+        <v>279</v>
+      </c>
+      <c r="P63">
+        <v>201800022</v>
+      </c>
+      <c r="Q63">
+        <v>1</v>
+      </c>
+      <c r="S63">
+        <v>1</v>
+      </c>
+      <c r="U63">
+        <v>1</v>
+      </c>
+      <c r="AR63">
+        <v>1</v>
+      </c>
+      <c r="AU63">
+        <v>1</v>
+      </c>
+      <c r="BE63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>299</v>
       </c>
       <c r="B64">
-        <v>201800173</v>
+        <v>201800024</v>
       </c>
       <c r="D64">
         <v>2</v>
@@ -5079,22 +5426,28 @@
         <v>171</v>
       </c>
       <c r="G64" t="s">
-        <v>297</v>
+        <v>294</v>
+      </c>
+      <c r="H64" t="s">
+        <v>300</v>
       </c>
       <c r="I64">
         <v>7.5</v>
       </c>
       <c r="J64" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="K64">
         <v>2022</v>
       </c>
       <c r="L64">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P64">
-        <v>201800171</v>
+        <v>201800022</v>
+      </c>
+      <c r="Q64">
+        <v>1</v>
       </c>
       <c r="S64">
         <v>1</v>
@@ -5112,127 +5465,154 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>300</v>
+        <v>258</v>
       </c>
       <c r="B65">
-        <v>201800025</v>
-      </c>
-      <c r="D65">
-        <v>2</v>
+        <v>201300007</v>
+      </c>
+      <c r="D65" t="s">
+        <v>25</v>
       </c>
       <c r="E65" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="F65" t="s">
         <v>171</v>
       </c>
       <c r="G65" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="H65" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="I65">
         <v>7.5</v>
       </c>
       <c r="J65" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="K65">
         <v>2022</v>
       </c>
-      <c r="L65">
-        <v>3</v>
-      </c>
-      <c r="N65" t="s">
-        <v>282</v>
-      </c>
-      <c r="P65">
-        <v>201800022</v>
-      </c>
-      <c r="Q65">
-        <v>1</v>
+      <c r="L65" t="s">
+        <v>154</v>
+      </c>
+      <c r="M65" t="s">
+        <v>205</v>
+      </c>
+      <c r="P65" t="s">
+        <v>303</v>
       </c>
       <c r="S65">
         <v>1</v>
       </c>
-      <c r="U65">
-        <v>1</v>
-      </c>
-      <c r="AR65">
-        <v>1</v>
-      </c>
-      <c r="AU65">
-        <v>1</v>
-      </c>
-      <c r="BE65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="AE65">
+        <v>1</v>
+      </c>
+      <c r="AK65">
+        <v>1</v>
+      </c>
+      <c r="AL65">
+        <v>1</v>
+      </c>
+      <c r="AN65">
+        <v>1</v>
+      </c>
+      <c r="AO65">
+        <v>1</v>
+      </c>
+      <c r="AS65">
+        <v>1</v>
+      </c>
+      <c r="AW65">
+        <v>1</v>
+      </c>
+      <c r="AY65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B66">
-        <v>201800024</v>
-      </c>
-      <c r="D66">
-        <v>2</v>
+        <v>202100060</v>
+      </c>
+      <c r="D66" t="s">
+        <v>25</v>
       </c>
       <c r="E66" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="F66" t="s">
         <v>171</v>
       </c>
       <c r="G66" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="H66" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="I66">
         <v>7.5</v>
       </c>
       <c r="J66" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="K66">
         <v>2022</v>
       </c>
-      <c r="L66">
-        <v>3</v>
-      </c>
-      <c r="P66">
-        <v>201800022</v>
-      </c>
-      <c r="Q66">
-        <v>1</v>
+      <c r="L66" t="s">
+        <v>187</v>
+      </c>
+      <c r="M66" t="s">
+        <v>205</v>
+      </c>
+      <c r="P66" t="s">
+        <v>307</v>
       </c>
       <c r="S66">
         <v>1</v>
       </c>
-      <c r="U66">
-        <v>1</v>
-      </c>
-      <c r="AR66">
-        <v>1</v>
-      </c>
-      <c r="AU66">
-        <v>1</v>
-      </c>
-      <c r="BE66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="T66">
+        <v>1</v>
+      </c>
+      <c r="AA66">
+        <v>1</v>
+      </c>
+      <c r="AE66">
+        <v>1</v>
+      </c>
+      <c r="AK66">
+        <v>1</v>
+      </c>
+      <c r="AL66">
+        <v>1</v>
+      </c>
+      <c r="AO66">
+        <v>1</v>
+      </c>
+      <c r="AW66">
+        <v>1</v>
+      </c>
+      <c r="AX66">
+        <v>1</v>
+      </c>
+      <c r="AY66">
+        <v>1</v>
+      </c>
+      <c r="BF66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>261</v>
+        <v>309</v>
       </c>
       <c r="B67">
-        <v>201300007</v>
+        <v>201300004</v>
       </c>
       <c r="D67" t="s">
         <v>25</v>
@@ -5244,16 +5624,16 @@
         <v>171</v>
       </c>
       <c r="G67" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="H67" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="I67">
         <v>7.5</v>
       </c>
       <c r="J67" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="K67">
         <v>2022</v>
@@ -5262,13 +5642,13 @@
         <v>154</v>
       </c>
       <c r="M67" t="s">
-        <v>208</v>
+        <v>205</v>
+      </c>
+      <c r="N67" t="s">
+        <v>108</v>
       </c>
       <c r="P67" t="s">
-        <v>306</v>
-      </c>
-      <c r="S67">
-        <v>1</v>
+        <v>171</v>
       </c>
       <c r="AE67">
         <v>1</v>
@@ -5276,15 +5656,15 @@
       <c r="AK67">
         <v>1</v>
       </c>
-      <c r="AL67">
-        <v>1</v>
-      </c>
-      <c r="AN67">
-        <v>1</v>
-      </c>
       <c r="AO67">
         <v>1</v>
       </c>
+      <c r="AQ67">
+        <v>1</v>
+      </c>
+      <c r="AS67">
+        <v>1</v>
+      </c>
       <c r="AW67">
         <v>1</v>
       </c>
@@ -5292,8 +5672,1254 @@
         <v>1</v>
       </c>
     </row>
+    <row r="68" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>312</v>
+      </c>
+      <c r="B68">
+        <v>200300176</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+      <c r="E68" t="s">
+        <v>84</v>
+      </c>
+      <c r="F68" t="s">
+        <v>171</v>
+      </c>
+      <c r="G68" t="s">
+        <v>313</v>
+      </c>
+      <c r="I68">
+        <v>7.5</v>
+      </c>
+      <c r="J68" t="s">
+        <v>256</v>
+      </c>
+      <c r="K68">
+        <v>2022</v>
+      </c>
+      <c r="L68">
+        <v>4</v>
+      </c>
+      <c r="P68" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="U68">
+        <v>1</v>
+      </c>
+      <c r="AR68">
+        <v>1</v>
+      </c>
+      <c r="BE68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>315</v>
+      </c>
+      <c r="B69">
+        <v>202000003</v>
+      </c>
+      <c r="D69" t="s">
+        <v>25</v>
+      </c>
+      <c r="E69" t="s">
+        <v>17</v>
+      </c>
+      <c r="F69" t="s">
+        <v>171</v>
+      </c>
+      <c r="G69" t="s">
+        <v>316</v>
+      </c>
+      <c r="H69" t="s">
+        <v>317</v>
+      </c>
+      <c r="I69">
+        <v>2.5</v>
+      </c>
+      <c r="J69" t="s">
+        <v>256</v>
+      </c>
+      <c r="K69">
+        <v>2022</v>
+      </c>
+      <c r="L69">
+        <v>1</v>
+      </c>
+      <c r="M69" t="s">
+        <v>318</v>
+      </c>
+      <c r="P69" t="s">
+        <v>171</v>
+      </c>
+      <c r="U69">
+        <v>1</v>
+      </c>
+      <c r="AR69">
+        <v>1</v>
+      </c>
+      <c r="BE69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>319</v>
+      </c>
+      <c r="B70">
+        <v>201000129</v>
+      </c>
+      <c r="D70">
+        <v>3</v>
+      </c>
+      <c r="E70" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" t="s">
+        <v>171</v>
+      </c>
+      <c r="G70" t="s">
+        <v>320</v>
+      </c>
+      <c r="I70">
+        <v>7.5</v>
+      </c>
+      <c r="J70" t="s">
+        <v>256</v>
+      </c>
+      <c r="K70">
+        <v>2022</v>
+      </c>
+      <c r="L70">
+        <v>4</v>
+      </c>
+      <c r="N70" t="s">
+        <v>321</v>
+      </c>
+      <c r="O70" t="s">
+        <v>323</v>
+      </c>
+      <c r="P70" t="s">
+        <v>322</v>
+      </c>
+      <c r="Q70">
+        <v>1</v>
+      </c>
+      <c r="S70">
+        <v>1</v>
+      </c>
+      <c r="U70">
+        <v>1</v>
+      </c>
+      <c r="AR70">
+        <v>1</v>
+      </c>
+      <c r="BE70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>326</v>
+      </c>
+      <c r="B71">
+        <v>201700012</v>
+      </c>
+      <c r="D71" t="s">
+        <v>25</v>
+      </c>
+      <c r="E71" t="s">
+        <v>17</v>
+      </c>
+      <c r="F71" t="s">
+        <v>171</v>
+      </c>
+      <c r="G71" t="s">
+        <v>179</v>
+      </c>
+      <c r="H71" t="s">
+        <v>324</v>
+      </c>
+      <c r="I71">
+        <v>15</v>
+      </c>
+      <c r="J71" t="s">
+        <v>256</v>
+      </c>
+      <c r="K71">
+        <v>2022</v>
+      </c>
+      <c r="L71" t="s">
+        <v>154</v>
+      </c>
+      <c r="P71" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q71">
+        <v>1</v>
+      </c>
+      <c r="S71">
+        <v>1</v>
+      </c>
+      <c r="U71">
+        <v>1</v>
+      </c>
+      <c r="V71">
+        <v>1</v>
+      </c>
+      <c r="X71">
+        <v>1</v>
+      </c>
+      <c r="AA71">
+        <v>1</v>
+      </c>
+      <c r="AE71">
+        <v>1</v>
+      </c>
+      <c r="AH71">
+        <v>1</v>
+      </c>
+      <c r="AK71">
+        <v>1</v>
+      </c>
+      <c r="AO71">
+        <v>1</v>
+      </c>
+      <c r="AQ71">
+        <v>1</v>
+      </c>
+      <c r="AR71">
+        <v>1</v>
+      </c>
+      <c r="AV71">
+        <v>1</v>
+      </c>
+      <c r="AW71">
+        <v>1</v>
+      </c>
+      <c r="AY71">
+        <v>1</v>
+      </c>
+      <c r="BE71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>325</v>
+      </c>
+      <c r="B72">
+        <v>201300052</v>
+      </c>
+      <c r="D72" t="s">
+        <v>25</v>
+      </c>
+      <c r="E72" t="s">
+        <v>17</v>
+      </c>
+      <c r="F72" t="s">
+        <v>171</v>
+      </c>
+      <c r="G72" t="s">
+        <v>327</v>
+      </c>
+      <c r="H72" t="s">
+        <v>327</v>
+      </c>
+      <c r="I72">
+        <v>7.5</v>
+      </c>
+      <c r="J72" t="s">
+        <v>256</v>
+      </c>
+      <c r="K72">
+        <v>2022</v>
+      </c>
+      <c r="L72" t="s">
+        <v>154</v>
+      </c>
+      <c r="N72" t="s">
+        <v>328</v>
+      </c>
+      <c r="P72" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q72">
+        <v>1</v>
+      </c>
+      <c r="AA72">
+        <v>1</v>
+      </c>
+      <c r="AE72">
+        <v>1</v>
+      </c>
+      <c r="AK72">
+        <v>1</v>
+      </c>
+      <c r="AO72">
+        <v>1</v>
+      </c>
+      <c r="AQ72">
+        <v>1</v>
+      </c>
+      <c r="AW72">
+        <v>1</v>
+      </c>
+      <c r="AY72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>329</v>
+      </c>
+      <c r="B73">
+        <v>202000005</v>
+      </c>
+      <c r="D73">
+        <v>3</v>
+      </c>
+      <c r="E73" t="s">
+        <v>84</v>
+      </c>
+      <c r="F73" t="s">
+        <v>171</v>
+      </c>
+      <c r="G73" t="s">
+        <v>330</v>
+      </c>
+      <c r="H73" t="s">
+        <v>331</v>
+      </c>
+      <c r="I73">
+        <v>7.5</v>
+      </c>
+      <c r="J73" t="s">
+        <v>256</v>
+      </c>
+      <c r="K73">
+        <v>2022</v>
+      </c>
+      <c r="L73" t="s">
+        <v>332</v>
+      </c>
+      <c r="M73" t="s">
+        <v>333</v>
+      </c>
+      <c r="P73" t="s">
+        <v>257</v>
+      </c>
+      <c r="AA73">
+        <v>1</v>
+      </c>
+      <c r="AE73">
+        <v>1</v>
+      </c>
+      <c r="AK73">
+        <v>1</v>
+      </c>
+      <c r="AN73">
+        <v>1</v>
+      </c>
+      <c r="AO73">
+        <v>1</v>
+      </c>
+      <c r="AQ73">
+        <v>1</v>
+      </c>
+      <c r="AY73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>334</v>
+      </c>
+      <c r="B74">
+        <v>202100002</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+      <c r="E74" t="s">
+        <v>84</v>
+      </c>
+      <c r="F74" t="s">
+        <v>171</v>
+      </c>
+      <c r="G74" t="s">
+        <v>335</v>
+      </c>
+      <c r="H74" t="s">
+        <v>336</v>
+      </c>
+      <c r="I74">
+        <v>3.75</v>
+      </c>
+      <c r="J74" t="s">
+        <v>256</v>
+      </c>
+      <c r="K74">
+        <v>2022</v>
+      </c>
+      <c r="L74">
+        <v>1</v>
+      </c>
+      <c r="P74" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="75" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>338</v>
+      </c>
+      <c r="B75">
+        <v>202000083</v>
+      </c>
+      <c r="D75" t="s">
+        <v>25</v>
+      </c>
+      <c r="E75" t="s">
+        <v>17</v>
+      </c>
+      <c r="F75" t="s">
+        <v>171</v>
+      </c>
+      <c r="G75" t="s">
+        <v>337</v>
+      </c>
+      <c r="H75" t="s">
+        <v>337</v>
+      </c>
+      <c r="I75">
+        <v>7.5</v>
+      </c>
+      <c r="J75" t="s">
+        <v>256</v>
+      </c>
+      <c r="K75">
+        <v>2022</v>
+      </c>
+      <c r="L75" t="s">
+        <v>154</v>
+      </c>
+      <c r="M75" t="s">
+        <v>188</v>
+      </c>
+      <c r="P75" t="s">
+        <v>171</v>
+      </c>
+      <c r="S75">
+        <v>1</v>
+      </c>
+      <c r="AQ75">
+        <v>1</v>
+      </c>
+      <c r="AR75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>339</v>
+      </c>
+      <c r="B76">
+        <v>200300004</v>
+      </c>
+      <c r="D76">
+        <v>3</v>
+      </c>
+      <c r="E76" t="s">
+        <v>84</v>
+      </c>
+      <c r="F76" t="s">
+        <v>171</v>
+      </c>
+      <c r="G76" t="s">
+        <v>340</v>
+      </c>
+      <c r="H76" t="s">
+        <v>341</v>
+      </c>
+      <c r="I76">
+        <v>7.5</v>
+      </c>
+      <c r="J76" t="s">
+        <v>256</v>
+      </c>
+      <c r="K76">
+        <v>2022</v>
+      </c>
+      <c r="L76">
+        <v>4</v>
+      </c>
+      <c r="N76" t="s">
+        <v>270</v>
+      </c>
+      <c r="P76" t="s">
+        <v>342</v>
+      </c>
+      <c r="Q76">
+        <v>1</v>
+      </c>
+      <c r="S76">
+        <v>1</v>
+      </c>
+      <c r="AO76">
+        <v>1</v>
+      </c>
+      <c r="AQ76">
+        <v>1</v>
+      </c>
+      <c r="AY76">
+        <v>1</v>
+      </c>
+      <c r="AZ76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>343</v>
+      </c>
+      <c r="B77">
+        <v>201900014</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77" t="s">
+        <v>84</v>
+      </c>
+      <c r="F77" t="s">
+        <v>171</v>
+      </c>
+      <c r="G77" t="s">
+        <v>344</v>
+      </c>
+      <c r="I77">
+        <v>7.5</v>
+      </c>
+      <c r="J77" t="s">
+        <v>256</v>
+      </c>
+      <c r="K77">
+        <v>2022</v>
+      </c>
+      <c r="L77">
+        <v>1</v>
+      </c>
+      <c r="N77" t="s">
+        <v>345</v>
+      </c>
+      <c r="P77" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q77">
+        <v>1</v>
+      </c>
+      <c r="S77">
+        <v>1</v>
+      </c>
+      <c r="U77">
+        <v>1</v>
+      </c>
+      <c r="AO77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>346</v>
+      </c>
+      <c r="B78">
+        <v>201300008</v>
+      </c>
+      <c r="D78" t="s">
+        <v>25</v>
+      </c>
+      <c r="E78" t="s">
+        <v>17</v>
+      </c>
+      <c r="F78" t="s">
+        <v>171</v>
+      </c>
+      <c r="G78" t="s">
+        <v>347</v>
+      </c>
+      <c r="H78" t="s">
+        <v>347</v>
+      </c>
+      <c r="I78">
+        <v>7.5</v>
+      </c>
+      <c r="J78" t="s">
+        <v>256</v>
+      </c>
+      <c r="K78">
+        <v>2022</v>
+      </c>
+      <c r="L78" t="s">
+        <v>154</v>
+      </c>
+      <c r="M78" t="s">
+        <v>205</v>
+      </c>
+      <c r="P78" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>186</v>
+      </c>
+      <c r="B79">
+        <v>202200015</v>
+      </c>
+      <c r="D79" t="s">
+        <v>25</v>
+      </c>
+      <c r="E79" t="s">
+        <v>17</v>
+      </c>
+      <c r="F79" t="s">
+        <v>171</v>
+      </c>
+      <c r="G79" t="s">
+        <v>348</v>
+      </c>
+      <c r="H79" t="s">
+        <v>348</v>
+      </c>
+      <c r="I79">
+        <v>2</v>
+      </c>
+      <c r="J79" t="s">
+        <v>256</v>
+      </c>
+      <c r="K79">
+        <v>2022</v>
+      </c>
+      <c r="L79" t="s">
+        <v>187</v>
+      </c>
+      <c r="P79" t="s">
+        <v>171</v>
+      </c>
+      <c r="U79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>349</v>
+      </c>
+      <c r="B80">
+        <v>201000091</v>
+      </c>
+      <c r="D80" t="s">
+        <v>25</v>
+      </c>
+      <c r="E80" t="s">
+        <v>17</v>
+      </c>
+      <c r="F80" t="s">
+        <v>171</v>
+      </c>
+      <c r="G80" t="s">
+        <v>350</v>
+      </c>
+      <c r="H80" t="s">
+        <v>350</v>
+      </c>
+      <c r="I80">
+        <v>7.5</v>
+      </c>
+      <c r="J80" t="s">
+        <v>256</v>
+      </c>
+      <c r="K80">
+        <v>2022</v>
+      </c>
+      <c r="L80" t="s">
+        <v>187</v>
+      </c>
+      <c r="M80" t="s">
+        <v>188</v>
+      </c>
+      <c r="P80" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="81" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>352</v>
+      </c>
+      <c r="B81">
+        <v>200800164</v>
+      </c>
+      <c r="D81" t="s">
+        <v>25</v>
+      </c>
+      <c r="E81" t="s">
+        <v>17</v>
+      </c>
+      <c r="F81" t="s">
+        <v>171</v>
+      </c>
+      <c r="G81" t="s">
+        <v>353</v>
+      </c>
+      <c r="H81" t="s">
+        <v>354</v>
+      </c>
+      <c r="I81">
+        <v>7.5</v>
+      </c>
+      <c r="J81" t="s">
+        <v>256</v>
+      </c>
+      <c r="K81">
+        <v>2022</v>
+      </c>
+      <c r="L81" t="s">
+        <v>154</v>
+      </c>
+      <c r="M81" t="s">
+        <v>355</v>
+      </c>
+      <c r="P81" t="s">
+        <v>171</v>
+      </c>
+      <c r="S81">
+        <v>1</v>
+      </c>
+      <c r="AO81">
+        <v>1</v>
+      </c>
+      <c r="AR81">
+        <v>1</v>
+      </c>
+      <c r="BE81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>356</v>
+      </c>
+      <c r="B82">
+        <v>200800167</v>
+      </c>
+      <c r="D82" t="s">
+        <v>25</v>
+      </c>
+      <c r="E82" t="s">
+        <v>17</v>
+      </c>
+      <c r="F82" t="s">
+        <v>171</v>
+      </c>
+      <c r="G82" t="s">
+        <v>357</v>
+      </c>
+      <c r="I82">
+        <v>7.5</v>
+      </c>
+      <c r="J82" t="s">
+        <v>256</v>
+      </c>
+      <c r="K82">
+        <v>2022</v>
+      </c>
+      <c r="L82" t="s">
+        <v>187</v>
+      </c>
+      <c r="M82" t="s">
+        <v>355</v>
+      </c>
+      <c r="P82" t="s">
+        <v>171</v>
+      </c>
+      <c r="AK82">
+        <v>1</v>
+      </c>
+      <c r="AO82">
+        <v>1</v>
+      </c>
+      <c r="AQ82">
+        <v>1</v>
+      </c>
+      <c r="AR82">
+        <v>1</v>
+      </c>
+      <c r="AY82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>358</v>
+      </c>
+      <c r="B83">
+        <v>200600024</v>
+      </c>
+      <c r="D83" t="s">
+        <v>25</v>
+      </c>
+      <c r="E83" t="s">
+        <v>17</v>
+      </c>
+      <c r="F83" t="s">
+        <v>171</v>
+      </c>
+      <c r="G83" t="s">
+        <v>359</v>
+      </c>
+      <c r="H83" t="s">
+        <v>287</v>
+      </c>
+      <c r="I83">
+        <v>7.5</v>
+      </c>
+      <c r="J83" t="s">
+        <v>256</v>
+      </c>
+      <c r="K83">
+        <v>2022</v>
+      </c>
+      <c r="L83" t="s">
+        <v>154</v>
+      </c>
+      <c r="M83" t="s">
+        <v>273</v>
+      </c>
+      <c r="P83" t="s">
+        <v>171</v>
+      </c>
+      <c r="S83">
+        <v>1</v>
+      </c>
+      <c r="U83">
+        <v>1</v>
+      </c>
+      <c r="AO83">
+        <v>1</v>
+      </c>
+      <c r="AR83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>360</v>
+      </c>
+      <c r="B84">
+        <v>200600028</v>
+      </c>
+      <c r="D84" t="s">
+        <v>25</v>
+      </c>
+      <c r="E84" t="s">
+        <v>17</v>
+      </c>
+      <c r="F84" t="s">
+        <v>171</v>
+      </c>
+      <c r="G84" t="s">
+        <v>361</v>
+      </c>
+      <c r="H84" t="s">
+        <v>362</v>
+      </c>
+      <c r="I84">
+        <v>7.5</v>
+      </c>
+      <c r="J84" t="s">
+        <v>256</v>
+      </c>
+      <c r="K84">
+        <v>2022</v>
+      </c>
+      <c r="L84" t="s">
+        <v>187</v>
+      </c>
+      <c r="M84" t="s">
+        <v>273</v>
+      </c>
+      <c r="P84" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="85" spans="1:57" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>363</v>
+      </c>
+      <c r="B85" t="s">
+        <v>363</v>
+      </c>
+      <c r="D85" t="s">
+        <v>25</v>
+      </c>
+      <c r="E85" t="s">
+        <v>17</v>
+      </c>
+      <c r="F85" t="s">
+        <v>171</v>
+      </c>
+      <c r="G85" t="s">
+        <v>266</v>
+      </c>
+      <c r="H85" t="s">
+        <v>364</v>
+      </c>
+      <c r="I85">
+        <v>7.5</v>
+      </c>
+      <c r="J85" t="s">
+        <v>256</v>
+      </c>
+      <c r="K85">
+        <v>2022</v>
+      </c>
+      <c r="L85">
+        <v>2</v>
+      </c>
+      <c r="N85" t="s">
+        <v>365</v>
+      </c>
+      <c r="P85" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q85">
+        <v>1</v>
+      </c>
+      <c r="S85">
+        <v>1</v>
+      </c>
+      <c r="U85">
+        <v>1</v>
+      </c>
+      <c r="AC85">
+        <v>1</v>
+      </c>
+      <c r="AO85">
+        <v>1</v>
+      </c>
+      <c r="AR85">
+        <v>1</v>
+      </c>
+      <c r="AY85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>367</v>
+      </c>
+      <c r="B86">
+        <v>201600008</v>
+      </c>
+      <c r="D86" t="s">
+        <v>25</v>
+      </c>
+      <c r="E86" t="s">
+        <v>17</v>
+      </c>
+      <c r="F86" t="s">
+        <v>171</v>
+      </c>
+      <c r="G86" t="s">
+        <v>368</v>
+      </c>
+      <c r="H86" t="s">
+        <v>369</v>
+      </c>
+      <c r="I86">
+        <v>7.5</v>
+      </c>
+      <c r="J86" t="s">
+        <v>256</v>
+      </c>
+      <c r="K86">
+        <v>2022</v>
+      </c>
+      <c r="L86" t="s">
+        <v>187</v>
+      </c>
+      <c r="M86" t="s">
+        <v>205</v>
+      </c>
+      <c r="P86" t="s">
+        <v>171</v>
+      </c>
+      <c r="S86">
+        <v>1</v>
+      </c>
+      <c r="T86">
+        <v>1</v>
+      </c>
+      <c r="U86">
+        <v>1</v>
+      </c>
+      <c r="AA86">
+        <v>1</v>
+      </c>
+      <c r="AE86">
+        <v>1</v>
+      </c>
+      <c r="AK86">
+        <v>1</v>
+      </c>
+      <c r="AM86">
+        <v>1</v>
+      </c>
+      <c r="AO86">
+        <v>1</v>
+      </c>
+      <c r="AQ86">
+        <v>1</v>
+      </c>
+      <c r="AR86">
+        <v>1</v>
+      </c>
+      <c r="AY86">
+        <v>1</v>
+      </c>
+      <c r="BE86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>370</v>
+      </c>
+      <c r="B87">
+        <v>202100010</v>
+      </c>
+      <c r="D87">
+        <v>3</v>
+      </c>
+      <c r="E87" t="s">
+        <v>84</v>
+      </c>
+      <c r="F87" t="s">
+        <v>171</v>
+      </c>
+      <c r="G87" t="s">
+        <v>244</v>
+      </c>
+      <c r="I87">
+        <v>7.5</v>
+      </c>
+      <c r="J87" t="s">
+        <v>256</v>
+      </c>
+      <c r="K87">
+        <v>2022</v>
+      </c>
+      <c r="L87">
+        <v>2</v>
+      </c>
+      <c r="M87" t="s">
+        <v>333</v>
+      </c>
+      <c r="N87" t="s">
+        <v>333</v>
+      </c>
+      <c r="S87">
+        <v>1</v>
+      </c>
+      <c r="Z87">
+        <v>1</v>
+      </c>
+      <c r="AC87">
+        <v>1</v>
+      </c>
+      <c r="AE87">
+        <v>1</v>
+      </c>
+      <c r="AK87">
+        <v>1</v>
+      </c>
+      <c r="AN87">
+        <v>1</v>
+      </c>
+      <c r="AO87">
+        <v>1</v>
+      </c>
+      <c r="AR87">
+        <v>1</v>
+      </c>
+      <c r="AY87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>371</v>
+      </c>
+      <c r="B88">
+        <v>202100050</v>
+      </c>
+      <c r="D88" t="s">
+        <v>25</v>
+      </c>
+      <c r="E88" t="s">
+        <v>17</v>
+      </c>
+      <c r="F88" t="s">
+        <v>171</v>
+      </c>
+      <c r="G88" t="s">
+        <v>167</v>
+      </c>
+      <c r="H88" t="s">
+        <v>372</v>
+      </c>
+      <c r="I88">
+        <v>7.5</v>
+      </c>
+      <c r="J88" t="s">
+        <v>256</v>
+      </c>
+      <c r="K88">
+        <v>2022</v>
+      </c>
+      <c r="L88" t="s">
+        <v>187</v>
+      </c>
+      <c r="M88" t="s">
+        <v>205</v>
+      </c>
+      <c r="P88" t="s">
+        <v>373</v>
+      </c>
+      <c r="S88">
+        <v>1</v>
+      </c>
+      <c r="AA88">
+        <v>1</v>
+      </c>
+      <c r="AE88">
+        <v>1</v>
+      </c>
+      <c r="AK88">
+        <v>1</v>
+      </c>
+      <c r="AL88">
+        <v>1</v>
+      </c>
+      <c r="AO88">
+        <v>1</v>
+      </c>
+      <c r="AR88">
+        <v>1</v>
+      </c>
+      <c r="AW88">
+        <v>1</v>
+      </c>
+      <c r="AY88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>374</v>
+      </c>
+      <c r="B89">
+        <v>201800051</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89" t="s">
+        <v>84</v>
+      </c>
+      <c r="F89" t="s">
+        <v>171</v>
+      </c>
+      <c r="G89" t="s">
+        <v>294</v>
+      </c>
+      <c r="H89" t="s">
+        <v>294</v>
+      </c>
+      <c r="I89">
+        <v>7.5</v>
+      </c>
+      <c r="J89" t="s">
+        <v>256</v>
+      </c>
+      <c r="K89">
+        <v>2022</v>
+      </c>
+      <c r="L89">
+        <v>1</v>
+      </c>
+      <c r="P89" t="s">
+        <v>171</v>
+      </c>
+      <c r="S89">
+        <v>1</v>
+      </c>
+      <c r="AO89">
+        <v>1</v>
+      </c>
+      <c r="AW89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>375</v>
+      </c>
+      <c r="B90">
+        <v>201100055</v>
+      </c>
+      <c r="D90" t="s">
+        <v>25</v>
+      </c>
+      <c r="E90" t="s">
+        <v>17</v>
+      </c>
+      <c r="F90" t="s">
+        <v>171</v>
+      </c>
+      <c r="G90" t="s">
+        <v>376</v>
+      </c>
+      <c r="H90" t="s">
+        <v>377</v>
+      </c>
+      <c r="I90">
+        <v>7.5</v>
+      </c>
+      <c r="J90" t="s">
+        <v>256</v>
+      </c>
+      <c r="K90">
+        <v>2022</v>
+      </c>
+      <c r="L90" t="s">
+        <v>154</v>
+      </c>
+      <c r="M90" t="s">
+        <v>273</v>
+      </c>
+      <c r="P90" t="s">
+        <v>171</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AZ67" xr:uid="{501E35CE-ACC9-4FC1-9D06-B7BA9C0949C0}"/>
+  <autoFilter ref="A1:AZ65" xr:uid="{501E35CE-ACC9-4FC1-9D06-B7BA9C0949C0}"/>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>